<commit_message>
fix false negatives due to invalid parameters lingering from a prior version of the sheet
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV-I_Carillon.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV-I_Carillon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\gsa-devel\piv-conformance-swing\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49A9D8D8-6644-44C9-A376-CDB954068450}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BA0C67-2DC4-44D2-83F4-E390B8B2C580}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="1830" windowWidth="26190" windowHeight="13845" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3776" uniqueCount="1309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3775" uniqueCount="1309">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -4823,17 +4823,17 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="13.75" style="4" customWidth="1"/>
-    <col min="2" max="2" width="57.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="57.35546875" style="4" customWidth="1"/>
     <col min="3" max="5" width="10.5" style="4" customWidth="1"/>
-    <col min="6" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="17" customWidth="1"/>
+    <col min="6" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A2" s="2">
         <v>8</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A3" s="3">
         <v>8.1</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>57</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>63</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>66</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>69</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>72</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>75</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>78</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>84</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>87</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A15" s="3">
         <v>8.1999999999999993</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>90</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="17" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>92</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>93</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>94</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>95</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>98</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="22" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>101</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>104</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>107</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>110</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>113</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>116</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>119</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>122</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>124</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>128</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A32" s="3">
         <v>8.3000000000000007</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>130</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>132</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="35" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>133</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="36" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>134</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="37" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>135</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="38" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>138</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="39" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>141</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="40" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>144</v>
       </c>
@@ -5153,7 +5153,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="41" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A41" s="3" t="s">
         <v>147</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A42" s="3" t="s">
         <v>150</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="43" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A43" s="3">
         <v>8.4</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="44" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A44" s="3" t="s">
         <v>151</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="45" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A45" s="3" t="s">
         <v>153</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="46" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A46" s="3" t="s">
         <v>154</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="47" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A47" s="3" t="s">
         <v>155</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="48" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A48" s="3" t="s">
         <v>156</v>
       </c>
@@ -5220,7 +5220,7 @@
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="49" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A49" s="3" t="s">
         <v>157</v>
       </c>
@@ -5231,7 +5231,7 @@
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
     </row>
-    <row r="50" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="50" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>158</v>
       </c>
@@ -5242,7 +5242,7 @@
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
     </row>
-    <row r="51" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="51" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A51" s="3" t="s">
         <v>159</v>
       </c>
@@ -5253,7 +5253,7 @@
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
     </row>
-    <row r="52" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="52" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A52" s="3" t="s">
         <v>160</v>
       </c>
@@ -5264,7 +5264,7 @@
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
     </row>
-    <row r="53" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="53" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A53" s="3">
         <v>8.5</v>
       </c>
@@ -5275,7 +5275,7 @@
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="54" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A54" s="3" t="s">
         <v>161</v>
       </c>
@@ -5286,7 +5286,7 @@
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
     </row>
-    <row r="55" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="55" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A55" s="3" t="s">
         <v>163</v>
       </c>
@@ -5297,7 +5297,7 @@
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="56" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A56" s="3" t="s">
         <v>164</v>
       </c>
@@ -5308,7 +5308,7 @@
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
     </row>
-    <row r="57" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="57" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A57" s="3" t="s">
         <v>165</v>
       </c>
@@ -5319,7 +5319,7 @@
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
     </row>
-    <row r="58" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="58" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A58" s="3" t="s">
         <v>166</v>
       </c>
@@ -5330,7 +5330,7 @@
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
     </row>
-    <row r="59" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="59" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A59" s="3" t="s">
         <v>169</v>
       </c>
@@ -5341,7 +5341,7 @@
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
     </row>
-    <row r="60" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="60" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A60" s="3" t="s">
         <v>172</v>
       </c>
@@ -5352,7 +5352,7 @@
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="61" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A61" s="3" t="s">
         <v>175</v>
       </c>
@@ -5363,7 +5363,7 @@
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
     </row>
-    <row r="62" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="62" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A62" s="3" t="s">
         <v>178</v>
       </c>
@@ -5374,7 +5374,7 @@
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
     </row>
-    <row r="63" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="63" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A63" s="3" t="s">
         <v>181</v>
       </c>
@@ -5385,7 +5385,7 @@
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
     </row>
-    <row r="64" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="64" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A64" s="3">
         <v>8.6</v>
       </c>
@@ -5396,7 +5396,7 @@
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
     </row>
-    <row r="65" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="65" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A65" s="3" t="s">
         <v>182</v>
       </c>
@@ -5407,7 +5407,7 @@
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="66" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A66" s="3" t="s">
         <v>184</v>
       </c>
@@ -5418,7 +5418,7 @@
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
     </row>
-    <row r="67" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="67" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A67" s="3" t="s">
         <v>185</v>
       </c>
@@ -5429,7 +5429,7 @@
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
     </row>
-    <row r="68" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="68" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A68" s="3" t="s">
         <v>186</v>
       </c>
@@ -5440,7 +5440,7 @@
       <c r="D68" s="16"/>
       <c r="E68" s="16"/>
     </row>
-    <row r="69" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="69" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A69" s="3" t="s">
         <v>187</v>
       </c>
@@ -5451,7 +5451,7 @@
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
     </row>
-    <row r="70" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="70" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A70" s="3" t="s">
         <v>190</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="31.5">
+    <row r="74" spans="1:5" ht="31.75">
       <c r="A74" s="3" t="s">
         <v>197</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="31.5">
+    <row r="85" spans="1:2" ht="31.75">
       <c r="A85" s="3" t="s">
         <v>208</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="31.5">
+    <row r="96" spans="1:2" ht="31.75">
       <c r="A96" s="3" t="s">
         <v>219</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="31.5">
+    <row r="114" spans="1:2" ht="31.75">
       <c r="A114" s="3" t="s">
         <v>244</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="28.5">
+    <row r="116" spans="1:2" ht="28.3">
       <c r="A116" s="3" t="s">
         <v>247</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="47.25">
+    <row r="121" spans="1:2" ht="47.6">
       <c r="A121" s="3" t="s">
         <v>256</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="63">
+    <row r="123" spans="1:2" ht="63.45">
       <c r="A123" s="3" t="s">
         <v>261</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="31.5">
+    <row r="142" spans="1:2" ht="31.75">
       <c r="A142" s="3" t="s">
         <v>284</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="31.5">
+    <row r="144" spans="1:2" ht="31.75">
       <c r="A144" s="3" t="s">
         <v>288</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="47.25">
+    <row r="145" spans="1:2" ht="31.75">
       <c r="A145" s="3" t="s">
         <v>290</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="47.25">
+    <row r="146" spans="1:2" ht="47.6">
       <c r="A146" s="3" t="s">
         <v>292</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="47.25">
+    <row r="149" spans="1:2" ht="47.6">
       <c r="A149" s="3" t="s">
         <v>298</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="63">
+    <row r="151" spans="1:2" ht="47.6">
       <c r="A151" s="3" t="s">
         <v>302</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="31.5">
+    <row r="152" spans="1:2" ht="31.75">
       <c r="A152" s="3" t="s">
         <v>304</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="31.5">
+    <row r="153" spans="1:2" ht="31.75">
       <c r="A153" s="3" t="s">
         <v>306</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="31.5">
+    <row r="161" spans="1:2" ht="31.75">
       <c r="A161" s="3" t="s">
         <v>314</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="31.5">
+    <row r="163" spans="1:2" ht="31.75">
       <c r="A163" s="3" t="s">
         <v>316</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="31.5">
+    <row r="164" spans="1:2" ht="31.75">
       <c r="A164" s="3" t="s">
         <v>317</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="47.25">
+    <row r="165" spans="1:2" ht="47.6">
       <c r="A165" s="3" t="s">
         <v>319</v>
       </c>
@@ -6238,7 +6238,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="31.5">
+    <row r="168" spans="1:2" ht="31.75">
       <c r="A168" s="3" t="s">
         <v>323</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="63">
+    <row r="170" spans="1:2" ht="47.6">
       <c r="A170" s="3" t="s">
         <v>327</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="31.5">
+    <row r="171" spans="1:2" ht="31.75">
       <c r="A171" s="3" t="s">
         <v>328</v>
       </c>
@@ -6270,7 +6270,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="31.5">
+    <row r="172" spans="1:2" ht="31.75">
       <c r="A172" s="3" t="s">
         <v>329</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="47.25">
+    <row r="184" spans="1:2" ht="47.6">
       <c r="A184" s="3" t="s">
         <v>319</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="31.5">
+    <row r="187" spans="1:2" ht="31.75">
       <c r="A187" s="3" t="s">
         <v>346</v>
       </c>
@@ -6406,7 +6406,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="63">
+    <row r="189" spans="1:2" ht="47.6">
       <c r="A189" s="3" t="s">
         <v>349</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="31.5">
+    <row r="190" spans="1:2" ht="31.75">
       <c r="A190" s="3" t="s">
         <v>350</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="31.5">
+    <row r="191" spans="1:2" ht="31.75">
       <c r="A191" s="3" t="s">
         <v>351</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="47.25">
+    <row r="197" spans="1:2" ht="47.6">
       <c r="A197" s="3" t="s">
         <v>361</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="47.25">
+    <row r="198" spans="1:2" ht="47.6">
       <c r="A198" s="3" t="s">
         <v>363</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="31.5">
+    <row r="201" spans="1:2" ht="31.75">
       <c r="A201" s="3" t="s">
         <v>368</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="31.5">
+    <row r="202" spans="1:2" ht="31.75">
       <c r="A202" s="3" t="s">
         <v>370</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="31.5">
+    <row r="215" spans="1:2" ht="31.75">
       <c r="A215" s="3" t="s">
         <v>395</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="47.25">
+    <row r="233" spans="1:2" ht="47.6">
       <c r="A233" s="3" t="s">
         <v>417</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="31.5">
+    <row r="235" spans="1:2" ht="31.75">
       <c r="A235" s="3" t="s">
         <v>423</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="31.5">
+    <row r="236" spans="1:2" ht="31.75">
       <c r="A236" s="3" t="s">
         <v>426</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="47.25">
+    <row r="239" spans="1:2" ht="47.6">
       <c r="A239" s="3" t="s">
         <v>435</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="47.25">
+    <row r="240" spans="1:2" ht="47.6">
       <c r="A240" s="3" t="s">
         <v>438</v>
       </c>
@@ -6822,7 +6822,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="78.75">
+    <row r="241" spans="1:2" ht="79.3">
       <c r="A241" s="3" t="s">
         <v>441</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="47.25">
+    <row r="242" spans="1:2" ht="47.6">
       <c r="A242" s="3" t="s">
         <v>444</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="78.75">
+    <row r="243" spans="1:2" ht="79.3">
       <c r="A243" s="3" t="s">
         <v>447</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="31.5">
+    <row r="244" spans="1:2" ht="31.75">
       <c r="A244" s="3" t="s">
         <v>450</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="47.25">
+    <row r="247" spans="1:2" ht="47.6">
       <c r="A247" s="3" t="s">
         <v>455</v>
       </c>
@@ -6886,7 +6886,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="31.5">
+    <row r="249" spans="1:2" ht="31.75">
       <c r="A249" s="3" t="s">
         <v>459</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="31.5">
+    <row r="250" spans="1:2" ht="31.75">
       <c r="A250" s="3" t="s">
         <v>461</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="31.5">
+    <row r="254" spans="1:2" ht="31.75">
       <c r="A254" s="3" t="s">
         <v>467</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="31.5">
+    <row r="255" spans="1:2" ht="31.75">
       <c r="A255" s="3" t="s">
         <v>469</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="31.5">
+    <row r="256" spans="1:2" ht="31.75">
       <c r="A256" s="3" t="s">
         <v>472</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="47.25">
+    <row r="257" spans="1:2" ht="47.6">
       <c r="A257" s="3" t="s">
         <v>474</v>
       </c>
@@ -6958,7 +6958,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="47.25">
+    <row r="258" spans="1:2" ht="47.6">
       <c r="A258" s="3" t="s">
         <v>477</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="63">
+    <row r="259" spans="1:2" ht="63.45">
       <c r="A259" s="3" t="s">
         <v>479</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="78.75">
+    <row r="260" spans="1:2" ht="79.3">
       <c r="A260" s="3" t="s">
         <v>481</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="78.75">
+    <row r="261" spans="1:2" ht="79.3">
       <c r="A261" s="3" t="s">
         <v>483</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="47.25">
+    <row r="262" spans="1:2" ht="47.6">
       <c r="A262" s="3" t="s">
         <v>486</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="47.25">
+    <row r="265" spans="1:2" ht="47.6">
       <c r="A265" s="3" t="s">
         <v>490</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="31.5">
+    <row r="267" spans="1:2" ht="31.75">
       <c r="A267" s="3" t="s">
         <v>492</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="31.5">
+    <row r="268" spans="1:2" ht="31.75">
       <c r="A268" s="3" t="s">
         <v>493</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="31.5">
+    <row r="272" spans="1:2" ht="31.75">
       <c r="A272" s="3" t="s">
         <v>497</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="31.5">
+    <row r="273" spans="1:2" ht="31.75">
       <c r="A273" s="3" t="s">
         <v>498</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="31.5">
+    <row r="274" spans="1:2" ht="31.75">
       <c r="A274" s="3" t="s">
         <v>499</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="47.25">
+    <row r="275" spans="1:2" ht="47.6">
       <c r="A275" s="3" t="s">
         <v>500</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="276" spans="1:2" ht="47.25">
+    <row r="276" spans="1:2" ht="47.6">
       <c r="A276" s="3" t="s">
         <v>501</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="277" spans="1:2" ht="63">
+    <row r="277" spans="1:2" ht="63.45">
       <c r="A277" s="3" t="s">
         <v>502</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="78.75">
+    <row r="278" spans="1:2" ht="79.3">
       <c r="A278" s="3" t="s">
         <v>503</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="78.75">
+    <row r="279" spans="1:2" ht="79.3">
       <c r="A279" s="3" t="s">
         <v>504</v>
       </c>
@@ -7134,7 +7134,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="280" spans="1:2" ht="47.25">
+    <row r="280" spans="1:2" ht="47.6">
       <c r="A280" s="3" t="s">
         <v>505</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="31.5">
+    <row r="283" spans="1:2" ht="31.75">
       <c r="A283" s="3" t="s">
         <v>507</v>
       </c>
@@ -7174,7 +7174,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="31.5">
+    <row r="285" spans="1:2" ht="31.75">
       <c r="A285" s="3" t="s">
         <v>511</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="47.25">
+    <row r="288" spans="1:2" ht="47.6">
       <c r="A288" s="3" t="s">
         <v>519</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="78.75">
+    <row r="291" spans="1:2" ht="79.3">
       <c r="A291" s="3" t="s">
         <v>527</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="47.25">
+    <row r="294" spans="1:2" ht="47.6">
       <c r="A294" s="3" t="s">
         <v>531</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="31.5">
+    <row r="296" spans="1:2" ht="31.75">
       <c r="A296" s="3" t="s">
         <v>533</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="31.5">
+    <row r="297" spans="1:2" ht="31.75">
       <c r="A297" s="3" t="s">
         <v>534</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="31.5">
+    <row r="301" spans="1:2" ht="31.75">
       <c r="A301" s="3" t="s">
         <v>538</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="31.5">
+    <row r="302" spans="1:2" ht="31.75">
       <c r="A302" s="3" t="s">
         <v>539</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="31.5">
+    <row r="303" spans="1:2" ht="31.75">
       <c r="A303" s="3" t="s">
         <v>540</v>
       </c>
@@ -7326,7 +7326,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="47.25">
+    <row r="304" spans="1:2" ht="47.6">
       <c r="A304" s="3" t="s">
         <v>541</v>
       </c>
@@ -7334,7 +7334,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="305" spans="1:2" ht="47.25">
+    <row r="305" spans="1:2" ht="47.6">
       <c r="A305" s="3" t="s">
         <v>542</v>
       </c>
@@ -7342,7 +7342,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="306" spans="1:2" ht="63">
+    <row r="306" spans="1:2" ht="63.45">
       <c r="A306" s="3" t="s">
         <v>543</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="307" spans="1:2" ht="78.75">
+    <row r="307" spans="1:2" ht="79.3">
       <c r="A307" s="3" t="s">
         <v>544</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="308" spans="1:2" ht="78.75">
+    <row r="308" spans="1:2" ht="79.3">
       <c r="A308" s="3" t="s">
         <v>545</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="47.25">
+    <row r="309" spans="1:2" ht="47.6">
       <c r="A309" s="3" t="s">
         <v>546</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="94.5">
+    <row r="313" spans="1:2" ht="95.15">
       <c r="A313" s="3" t="s">
         <v>548</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="31.5">
+    <row r="314" spans="1:2" ht="31.75">
       <c r="A314" s="3" t="s">
         <v>550</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="31.5">
+    <row r="320" spans="1:2" ht="31.75">
       <c r="A320" s="3" t="s">
         <v>564</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="31.5">
+    <row r="324" spans="1:2" ht="31.75">
       <c r="A324" s="3" t="s">
         <v>575</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="326" spans="1:2" ht="31.5">
+    <row r="326" spans="1:2" ht="31.75">
       <c r="A326" s="3" t="s">
         <v>581</v>
       </c>
@@ -7518,7 +7518,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="63">
+    <row r="328" spans="1:2" ht="63.45">
       <c r="A328" s="3" t="s">
         <v>587</v>
       </c>
@@ -7526,7 +7526,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="329" spans="1:2" ht="47.25">
+    <row r="329" spans="1:2" ht="47.6">
       <c r="A329" s="3" t="s">
         <v>589</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="331" spans="1:2" ht="31.5">
+    <row r="331" spans="1:2" ht="31.75">
       <c r="A331" s="3" t="s">
         <v>593</v>
       </c>
@@ -7550,7 +7550,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="332" spans="1:2" ht="31.5">
+    <row r="332" spans="1:2" ht="31.75">
       <c r="A332" s="3" t="s">
         <v>596</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="31.5">
+    <row r="339" spans="1:2" ht="31.75">
       <c r="A339" s="3" t="s">
         <v>610</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="94.5">
+    <row r="344" spans="1:2" ht="95.15">
       <c r="A344" s="3" t="s">
         <v>618</v>
       </c>
@@ -7654,7 +7654,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="31.5">
+    <row r="345" spans="1:2" ht="31.75">
       <c r="A345" s="3" t="s">
         <v>619</v>
       </c>
@@ -7702,7 +7702,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="31.5">
+    <row r="351" spans="1:2" ht="31.75">
       <c r="A351" s="3" t="s">
         <v>631</v>
       </c>
@@ -7710,7 +7710,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="31.5">
+    <row r="352" spans="1:2" ht="31.75">
       <c r="A352" s="3" t="s">
         <v>633</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="31.5">
+    <row r="353" spans="1:2" ht="31.75">
       <c r="A353" s="3" t="s">
         <v>635</v>
       </c>
@@ -7726,7 +7726,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="354" spans="1:2" ht="31.5">
+    <row r="354" spans="1:2" ht="47.6">
       <c r="A354" s="3" t="s">
         <v>637</v>
       </c>
@@ -7782,7 +7782,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="31.5">
+    <row r="361" spans="1:2" ht="31.75">
       <c r="A361" s="3" t="s">
         <v>646</v>
       </c>
@@ -7822,7 +7822,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="78.75">
+    <row r="366" spans="1:2" ht="79.3">
       <c r="A366" s="3" t="s">
         <v>650</v>
       </c>
@@ -7830,7 +7830,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="31.5">
+    <row r="367" spans="1:2" ht="31.75">
       <c r="A367" s="3" t="s">
         <v>652</v>
       </c>
@@ -7862,7 +7862,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="31.5">
+    <row r="371" spans="1:2" ht="31.75">
       <c r="A371" s="3" t="s">
         <v>658</v>
       </c>
@@ -7870,7 +7870,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="31.5">
+    <row r="372" spans="1:2" ht="31.75">
       <c r="A372" s="3" t="s">
         <v>660</v>
       </c>
@@ -7886,7 +7886,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="31.5">
+    <row r="374" spans="1:2" ht="31.75">
       <c r="A374" s="3" t="s">
         <v>665</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="31.5">
+    <row r="375" spans="1:2" ht="31.75">
       <c r="A375" s="3" t="s">
         <v>667</v>
       </c>
@@ -7902,7 +7902,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="31.5">
+    <row r="376" spans="1:2" ht="47.6">
       <c r="A376" s="3" t="s">
         <v>669</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="383" spans="1:2" ht="31.5">
+    <row r="383" spans="1:2" ht="31.75">
       <c r="A383" s="3" t="s">
         <v>676</v>
       </c>
@@ -7998,7 +7998,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="388" spans="1:2" ht="78.75">
+    <row r="388" spans="1:2" ht="79.3">
       <c r="A388" s="3" t="s">
         <v>680</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="389" spans="1:2" ht="31.5">
+    <row r="389" spans="1:2" ht="31.75">
       <c r="A389" s="3" t="s">
         <v>681</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="396" spans="1:2" ht="31.5">
+    <row r="396" spans="1:2" ht="31.75">
       <c r="A396" s="3" t="s">
         <v>691</v>
       </c>
@@ -8086,7 +8086,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="399" spans="1:2" ht="31.5">
+    <row r="399" spans="1:2" ht="31.75">
       <c r="A399" s="3" t="s">
         <v>698</v>
       </c>
@@ -8126,7 +8126,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="404" spans="1:2" ht="31.5">
+    <row r="404" spans="1:2" ht="31.75">
       <c r="A404" s="3" t="s">
         <v>707</v>
       </c>
@@ -8150,7 +8150,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="31.5">
+    <row r="407" spans="1:2" ht="31.75">
       <c r="A407" s="3" t="s">
         <v>710</v>
       </c>
@@ -8166,7 +8166,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="63">
+    <row r="409" spans="1:2" ht="63.45">
       <c r="A409" s="3" t="s">
         <v>712</v>
       </c>
@@ -8174,7 +8174,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="410" spans="1:2" ht="47.25">
+    <row r="410" spans="1:2" ht="47.6">
       <c r="A410" s="3" t="s">
         <v>713</v>
       </c>
@@ -8190,7 +8190,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="412" spans="1:2" ht="31.5">
+    <row r="412" spans="1:2" ht="31.75">
       <c r="A412" s="3" t="s">
         <v>716</v>
       </c>
@@ -8246,7 +8246,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="419" spans="1:2" ht="31.5">
+    <row r="419" spans="1:2" ht="31.75">
       <c r="A419" s="3" t="s">
         <v>723</v>
       </c>
@@ -8342,7 +8342,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="431" spans="1:2" ht="78.75">
+    <row r="431" spans="1:2" ht="79.3">
       <c r="A431" s="3" t="s">
         <v>732</v>
       </c>
@@ -8350,7 +8350,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="432" spans="1:2" ht="31.5">
+    <row r="432" spans="1:2" ht="31.75">
       <c r="A432" s="3" t="s">
         <v>733</v>
       </c>
@@ -8406,7 +8406,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="439" spans="1:2" ht="31.5">
+    <row r="439" spans="1:2" ht="31.75">
       <c r="A439" s="3" t="s">
         <v>742</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="440" spans="1:2" ht="47.25">
+    <row r="440" spans="1:2" ht="47.6">
       <c r="A440" s="3" t="s">
         <v>744</v>
       </c>
@@ -8478,7 +8478,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="448" spans="1:2" ht="31.5">
+    <row r="448" spans="1:2" ht="31.75">
       <c r="A448" s="3" t="s">
         <v>753</v>
       </c>
@@ -8517,22 +8517,24 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G472"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:XFD49"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="14.25" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.2109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="12" style="4" customWidth="1"/>
-    <col min="3" max="3" width="43.75" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.125" style="34" customWidth="1"/>
-    <col min="6" max="6" width="84.625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="80.875" style="31" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="34" customWidth="1"/>
+    <col min="6" max="6" width="84.640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="80.85546875" style="31" customWidth="1"/>
     <col min="8" max="1026" width="8.5" style="17" customWidth="1"/>
     <col min="1027" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="30" customFormat="1" ht="18.75">
+    <row r="1" spans="1:7" s="30" customFormat="1" ht="18.45">
       <c r="A1" s="35" t="s">
         <v>52</v>
       </c>
@@ -17051,16 +17053,18 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AMK6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="45.125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="4" customWidth="1"/>
-    <col min="4" max="5" width="81.375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.640625" style="4" customWidth="1"/>
+    <col min="4" max="5" width="81.35546875" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -17138,15 +17142,13 @@
       <c r="D4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>756</v>
-      </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="3" t="s">
         <v>764</v>
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="126">
+    <row r="5" spans="1:7" ht="126.9">
       <c r="A5" s="3" t="s">
         <v>68</v>
       </c>
@@ -17198,19 +17200,19 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AMK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G55"/>
+    <sheetView showGridLines="0" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="68.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="100" style="4" customWidth="1"/>
-    <col min="5" max="6" width="22.875" style="4" customWidth="1"/>
+    <col min="5" max="6" width="22.85546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="20" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -17351,7 +17353,7 @@
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="31.5">
+    <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
         <v>784</v>
       </c>
@@ -17904,7 +17906,7 @@
       </c>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" ht="63">
+    <row r="37" spans="1:7" ht="63.45">
       <c r="A37" s="6" t="s">
         <v>246</v>
       </c>
@@ -17925,7 +17927,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="31.5">
+    <row r="38" spans="1:7" ht="31.75">
       <c r="A38" s="6" t="s">
         <v>509</v>
       </c>
@@ -18001,7 +18003,7 @@
       </c>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:7" ht="47.25">
+    <row r="42" spans="1:7" ht="47.6">
       <c r="A42" s="6" t="s">
         <v>263</v>
       </c>
@@ -18285,19 +18287,19 @@
       <selection sqref="A1:D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="47.375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="4" customWidth="1"/>
-    <col min="4" max="5" width="80.875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="47.35546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="4" customWidth="1"/>
+    <col min="4" max="5" width="80.85546875" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="17" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="22" customFormat="1" ht="30.95" customHeight="1">
+    <row r="1" spans="1:256" s="22" customFormat="1" ht="31" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>756</v>
       </c>
@@ -18569,7 +18571,7 @@
       <c r="IU1" s="21"/>
       <c r="IV1" s="21"/>
     </row>
-    <row r="2" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>834</v>
       </c>
@@ -18588,7 +18590,7 @@
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>837</v>
       </c>
@@ -18607,7 +18609,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>839</v>
       </c>
@@ -18645,7 +18647,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>843</v>
       </c>
@@ -18664,7 +18666,7 @@
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>846</v>
       </c>
@@ -18683,7 +18685,7 @@
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>849</v>
       </c>
@@ -18721,7 +18723,7 @@
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>855</v>
       </c>
@@ -18740,7 +18742,7 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>857</v>
       </c>
@@ -18759,7 +18761,7 @@
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>859</v>
       </c>
@@ -18797,7 +18799,7 @@
       </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>864</v>
       </c>
@@ -18816,7 +18818,7 @@
       </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>866</v>
       </c>
@@ -18873,7 +18875,7 @@
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>868</v>
       </c>
@@ -18892,7 +18894,7 @@
       </c>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>870</v>
       </c>
@@ -18911,7 +18913,7 @@
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>872</v>
       </c>
@@ -18930,7 +18932,7 @@
       </c>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>874</v>
       </c>
@@ -18949,7 +18951,7 @@
       </c>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="22" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>877</v>
       </c>
@@ -18968,7 +18970,7 @@
       </c>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>879</v>
       </c>
@@ -18987,7 +18989,7 @@
       </c>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>881</v>
       </c>
@@ -19006,7 +19008,7 @@
       </c>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>883</v>
       </c>
@@ -19025,7 +19027,7 @@
       </c>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>886</v>
       </c>
@@ -19044,7 +19046,7 @@
       </c>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>888</v>
       </c>
@@ -19063,7 +19065,7 @@
       </c>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>891</v>
       </c>
@@ -19082,7 +19084,7 @@
       </c>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>893</v>
       </c>
@@ -19101,7 +19103,7 @@
       </c>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>895</v>
       </c>
@@ -19120,7 +19122,7 @@
       </c>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>897</v>
       </c>
@@ -19139,7 +19141,7 @@
       </c>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>900</v>
       </c>
@@ -19158,7 +19160,7 @@
       </c>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>903</v>
       </c>
@@ -19177,7 +19179,7 @@
       </c>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A34" s="6" t="s">
         <v>906</v>
       </c>
@@ -19196,7 +19198,7 @@
       </c>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="35" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A35" s="6" t="s">
         <v>909</v>
       </c>
@@ -19215,7 +19217,7 @@
       </c>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="36" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A36" s="6" t="s">
         <v>912</v>
       </c>
@@ -19234,7 +19236,7 @@
       </c>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="37" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>915</v>
       </c>
@@ -19253,7 +19255,7 @@
       </c>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="38" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A38" s="6" t="s">
         <v>918</v>
       </c>
@@ -19272,7 +19274,7 @@
       </c>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="39" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A39" s="6" t="s">
         <v>921</v>
       </c>
@@ -19291,7 +19293,7 @@
       </c>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" ht="30.95" customHeight="1">
+    <row r="40" spans="1:7" ht="31" customHeight="1">
       <c r="A40" s="6" t="s">
         <v>924</v>
       </c>
@@ -19327,7 +19329,7 @@
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A42" s="6" t="s">
         <v>931</v>
       </c>
@@ -19344,7 +19346,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:7" ht="30.95" customHeight="1">
+    <row r="43" spans="1:7" ht="31" customHeight="1">
       <c r="A43" s="6" t="s">
         <v>934</v>
       </c>
@@ -19382,7 +19384,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="45" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A45" s="6" t="s">
         <v>942</v>
       </c>
@@ -19435,7 +19437,7 @@
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="48" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A48" s="6" t="s">
         <v>952</v>
       </c>
@@ -19452,7 +19454,7 @@
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:256" s="29" customFormat="1" ht="31.5">
+    <row r="49" spans="1:256" s="29" customFormat="1" ht="31.75">
       <c r="A49" s="53" t="s">
         <v>955</v>
       </c>
@@ -19748,21 +19750,21 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="33.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="44.375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="41.375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="44.35546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41.35546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.640625" style="4" customWidth="1"/>
     <col min="7" max="7" width="29" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="17" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A1" s="53" t="s">
         <v>756</v>
       </c>
@@ -20228,7 +20230,7 @@
       <c r="F24" s="66"/>
       <c r="G24" s="66"/>
     </row>
-    <row r="25" spans="1:7" ht="45">
+    <row r="25" spans="1:7" ht="43.75">
       <c r="A25" s="66" t="s">
         <v>1211</v>
       </c>
@@ -20245,7 +20247,7 @@
       <c r="F25" s="66"/>
       <c r="G25" s="66"/>
     </row>
-    <row r="26" spans="1:7" ht="30">
+    <row r="26" spans="1:7" ht="29.15">
       <c r="A26" s="66" t="s">
         <v>1260</v>
       </c>
@@ -20262,7 +20264,7 @@
       <c r="F26" s="66"/>
       <c r="G26" s="66"/>
     </row>
-    <row r="27" spans="1:7" ht="30">
+    <row r="27" spans="1:7" ht="29.15">
       <c r="A27" s="66" t="s">
         <v>1263</v>
       </c>
@@ -20279,7 +20281,7 @@
       <c r="F27" s="66"/>
       <c r="G27" s="66"/>
     </row>
-    <row r="28" spans="1:7" ht="30">
+    <row r="28" spans="1:7" ht="29.15">
       <c r="A28" s="66" t="s">
         <v>1266</v>
       </c>
@@ -20296,7 +20298,7 @@
       <c r="F28" s="66"/>
       <c r="G28" s="66"/>
     </row>
-    <row r="29" spans="1:7" ht="30">
+    <row r="29" spans="1:7" ht="29.15">
       <c r="A29" s="66" t="s">
         <v>1269</v>
       </c>
@@ -20313,7 +20315,7 @@
       <c r="F29" s="66"/>
       <c r="G29" s="66"/>
     </row>
-    <row r="30" spans="1:7" ht="30">
+    <row r="30" spans="1:7" ht="29.15">
       <c r="A30" s="66" t="s">
         <v>1272</v>
       </c>
@@ -20348,15 +20350,15 @@
       <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="54.625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="4" customWidth="1"/>
-    <col min="4" max="5" width="75.625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="54.640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="4" customWidth="1"/>
+    <col min="4" max="5" width="75.640625" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="17" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -20421,7 +20423,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="63">
+    <row r="4" spans="1:7" ht="63.45">
       <c r="A4" s="5" t="s">
         <v>1004</v>
       </c>
@@ -20454,23 +20456,23 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="53.375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="53.35546875" style="18" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="18" customWidth="1"/>
     <col min="4" max="4" width="44.5" style="18" customWidth="1"/>
-    <col min="5" max="5" width="31.875" style="18" customWidth="1"/>
-    <col min="6" max="6" width="11.875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="18" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="18" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="18" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="18" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="25" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:256" s="25" customFormat="1" ht="17.149999999999999" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>756</v>
       </c>
@@ -20761,7 +20763,7 @@
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>627</v>
       </c>
@@ -20780,7 +20782,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>557</v>
       </c>
@@ -20799,7 +20801,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>560</v>
       </c>
@@ -20818,7 +20820,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>563</v>
       </c>
@@ -20837,7 +20839,7 @@
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:256" ht="315">
+    <row r="7" spans="1:256" ht="301.3">
       <c r="A7" s="6" t="s">
         <v>566</v>
       </c>
@@ -20860,7 +20862,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="8" spans="1:256" ht="31.5">
+    <row r="8" spans="1:256" ht="31.75">
       <c r="A8" s="6" t="s">
         <v>571</v>
       </c>
@@ -20917,7 +20919,7 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>580</v>
       </c>
@@ -20936,7 +20938,7 @@
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:256" ht="33.6" customHeight="1">
+    <row r="12" spans="1:256" ht="33.65" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>583</v>
       </c>
@@ -21098,7 +21100,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="20" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>697</v>
       </c>
@@ -21163,7 +21165,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="23" spans="1:256" s="33" customFormat="1" ht="31.5">
+    <row r="23" spans="1:256" s="33" customFormat="1" ht="31.75">
       <c r="A23" s="6" t="s">
         <v>1071</v>
       </c>
@@ -21963,7 +21965,7 @@
       <c r="IU25" s="32"/>
       <c r="IV25" s="32"/>
     </row>
-    <row r="26" spans="1:256" s="33" customFormat="1" ht="31.5">
+    <row r="26" spans="1:256" s="33" customFormat="1" ht="31.75">
       <c r="A26" s="6" t="s">
         <v>1067</v>
       </c>
@@ -22511,19 +22513,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="20" customWidth="1"/>
-    <col min="2" max="2" width="53.375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="53.35546875" style="17" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="17" customWidth="1"/>
     <col min="4" max="5" width="44.5" style="17" customWidth="1"/>
-    <col min="6" max="6" width="11.875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="17" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="17" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="17" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="22" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:256" s="22" customFormat="1" ht="17.149999999999999" customHeight="1">
       <c r="A1" s="51" t="s">
         <v>756</v>
       </c>
@@ -22795,7 +22797,7 @@
       <c r="IU1" s="21"/>
       <c r="IV1" s="21"/>
     </row>
-    <row r="2" spans="1:256" ht="31.5">
+    <row r="2" spans="1:256" ht="31.75">
       <c r="A2" s="52" t="s">
         <v>1200</v>
       </c>
@@ -22816,7 +22818,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="31.5">
+    <row r="3" spans="1:256" ht="31.75">
       <c r="A3" s="52" t="s">
         <v>1284</v>
       </c>
@@ -22837,7 +22839,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:256" ht="31.5">
+    <row r="4" spans="1:256" ht="31.75">
       <c r="A4" s="6" t="s">
         <v>1287</v>
       </c>

</xml_diff>

<commit_message>
Updated test section 11.7 with CHUID OID
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV-I_Carillon.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV-I_Carillon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\gsa-devel\piv-conformance-swing\conformancelib\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BA0C67-2DC4-44D2-83F4-E390B8B2C580}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9391F86A-6016-4C3F-8BB4-7AEE3AB495D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="1815" windowWidth="26190" windowHeight="13845" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3775" uniqueCount="1309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3769" uniqueCount="1309">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -4823,17 +4823,17 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="57.35546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.75" style="4" customWidth="1"/>
+    <col min="2" max="2" width="57.375" style="4" customWidth="1"/>
     <col min="3" max="5" width="10.5" style="4" customWidth="1"/>
-    <col min="6" max="256" width="8.85546875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.85546875" style="17" customWidth="1"/>
+    <col min="6" max="256" width="8.875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.875" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="1" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="2" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="2">
         <v>8</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="3" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="3">
         <v>8.1</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="4" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>57</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="5" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="6" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>63</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="7" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>66</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="8" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>69</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="9" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>72</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="10" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>75</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="11" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>78</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="12" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="13" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>84</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="14" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>87</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="15" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="3">
         <v>8.1999999999999993</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="16" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>90</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="17" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>92</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="18" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>93</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="19" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>94</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="20" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>95</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="21" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>98</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="22" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>101</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="23" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>104</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="24" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>107</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="25" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>110</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="26" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>113</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="27" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>116</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="28" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>119</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="29" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>122</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="30" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>124</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="31" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>128</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="17.149999999999999" customHeight="1">
+    <row r="32" spans="1:2" ht="17.100000000000001" customHeight="1">
       <c r="A32" s="3">
         <v>8.3000000000000007</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="33" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>130</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="34" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>132</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="35" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>133</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="36" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>134</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="37" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>135</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="38" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>138</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="39" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>141</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="40" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>144</v>
       </c>
@@ -5153,7 +5153,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="41" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A41" s="3" t="s">
         <v>147</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="42" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A42" s="3" t="s">
         <v>150</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="43" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A43" s="3">
         <v>8.4</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="44" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A44" s="3" t="s">
         <v>151</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="45" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="3" t="s">
         <v>153</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="46" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A46" s="3" t="s">
         <v>154</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="47" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A47" s="3" t="s">
         <v>155</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="48" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="3" t="s">
         <v>156</v>
       </c>
@@ -5220,7 +5220,7 @@
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
     </row>
-    <row r="49" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="49" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A49" s="3" t="s">
         <v>157</v>
       </c>
@@ -5231,7 +5231,7 @@
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
     </row>
-    <row r="50" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="50" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>158</v>
       </c>
@@ -5242,7 +5242,7 @@
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
     </row>
-    <row r="51" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="51" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A51" s="3" t="s">
         <v>159</v>
       </c>
@@ -5253,7 +5253,7 @@
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
     </row>
-    <row r="52" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="52" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A52" s="3" t="s">
         <v>160</v>
       </c>
@@ -5264,7 +5264,7 @@
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
     </row>
-    <row r="53" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="53" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A53" s="3">
         <v>8.5</v>
       </c>
@@ -5275,7 +5275,7 @@
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="54" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A54" s="3" t="s">
         <v>161</v>
       </c>
@@ -5286,7 +5286,7 @@
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
     </row>
-    <row r="55" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="55" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A55" s="3" t="s">
         <v>163</v>
       </c>
@@ -5297,7 +5297,7 @@
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
     </row>
-    <row r="56" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="56" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A56" s="3" t="s">
         <v>164</v>
       </c>
@@ -5308,7 +5308,7 @@
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
     </row>
-    <row r="57" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="57" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A57" s="3" t="s">
         <v>165</v>
       </c>
@@ -5319,7 +5319,7 @@
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
     </row>
-    <row r="58" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="58" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A58" s="3" t="s">
         <v>166</v>
       </c>
@@ -5330,7 +5330,7 @@
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
     </row>
-    <row r="59" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="59" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A59" s="3" t="s">
         <v>169</v>
       </c>
@@ -5341,7 +5341,7 @@
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
     </row>
-    <row r="60" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="60" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A60" s="3" t="s">
         <v>172</v>
       </c>
@@ -5352,7 +5352,7 @@
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
     </row>
-    <row r="61" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="61" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A61" s="3" t="s">
         <v>175</v>
       </c>
@@ -5363,7 +5363,7 @@
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
     </row>
-    <row r="62" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="62" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A62" s="3" t="s">
         <v>178</v>
       </c>
@@ -5374,7 +5374,7 @@
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
     </row>
-    <row r="63" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="63" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A63" s="3" t="s">
         <v>181</v>
       </c>
@@ -5385,7 +5385,7 @@
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
     </row>
-    <row r="64" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="64" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A64" s="3">
         <v>8.6</v>
       </c>
@@ -5396,7 +5396,7 @@
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
     </row>
-    <row r="65" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="65" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A65" s="3" t="s">
         <v>182</v>
       </c>
@@ -5407,7 +5407,7 @@
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
     </row>
-    <row r="66" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="66" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A66" s="3" t="s">
         <v>184</v>
       </c>
@@ -5418,7 +5418,7 @@
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
     </row>
-    <row r="67" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="67" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A67" s="3" t="s">
         <v>185</v>
       </c>
@@ -5429,7 +5429,7 @@
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
     </row>
-    <row r="68" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="68" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A68" s="3" t="s">
         <v>186</v>
       </c>
@@ -5440,7 +5440,7 @@
       <c r="D68" s="16"/>
       <c r="E68" s="16"/>
     </row>
-    <row r="69" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="69" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A69" s="3" t="s">
         <v>187</v>
       </c>
@@ -5451,7 +5451,7 @@
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
     </row>
-    <row r="70" spans="1:5" ht="17.149999999999999" customHeight="1">
+    <row r="70" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A70" s="3" t="s">
         <v>190</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="31.75">
+    <row r="74" spans="1:5" ht="31.5">
       <c r="A74" s="3" t="s">
         <v>197</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="31.75">
+    <row r="85" spans="1:2" ht="31.5">
       <c r="A85" s="3" t="s">
         <v>208</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="31.75">
+    <row r="96" spans="1:2" ht="31.5">
       <c r="A96" s="3" t="s">
         <v>219</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="31.75">
+    <row r="114" spans="1:2" ht="31.5">
       <c r="A114" s="3" t="s">
         <v>244</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="28.3">
+    <row r="116" spans="1:2" ht="28.5">
       <c r="A116" s="3" t="s">
         <v>247</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="47.6">
+    <row r="121" spans="1:2" ht="47.25">
       <c r="A121" s="3" t="s">
         <v>256</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="63.45">
+    <row r="123" spans="1:2" ht="63">
       <c r="A123" s="3" t="s">
         <v>261</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="31.75">
+    <row r="142" spans="1:2" ht="31.5">
       <c r="A142" s="3" t="s">
         <v>284</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="31.75">
+    <row r="144" spans="1:2" ht="31.5">
       <c r="A144" s="3" t="s">
         <v>288</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="31.75">
+    <row r="145" spans="1:2" ht="47.25">
       <c r="A145" s="3" t="s">
         <v>290</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="47.6">
+    <row r="146" spans="1:2" ht="47.25">
       <c r="A146" s="3" t="s">
         <v>292</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="47.6">
+    <row r="149" spans="1:2" ht="47.25">
       <c r="A149" s="3" t="s">
         <v>298</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="47.6">
+    <row r="151" spans="1:2" ht="63">
       <c r="A151" s="3" t="s">
         <v>302</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="31.75">
+    <row r="152" spans="1:2" ht="31.5">
       <c r="A152" s="3" t="s">
         <v>304</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="31.75">
+    <row r="153" spans="1:2" ht="31.5">
       <c r="A153" s="3" t="s">
         <v>306</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="31.75">
+    <row r="161" spans="1:2" ht="31.5">
       <c r="A161" s="3" t="s">
         <v>314</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="31.75">
+    <row r="163" spans="1:2" ht="31.5">
       <c r="A163" s="3" t="s">
         <v>316</v>
       </c>
@@ -6206,7 +6206,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="31.75">
+    <row r="164" spans="1:2" ht="31.5">
       <c r="A164" s="3" t="s">
         <v>317</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="47.6">
+    <row r="165" spans="1:2" ht="47.25">
       <c r="A165" s="3" t="s">
         <v>319</v>
       </c>
@@ -6238,7 +6238,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="31.75">
+    <row r="168" spans="1:2" ht="31.5">
       <c r="A168" s="3" t="s">
         <v>323</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="47.6">
+    <row r="170" spans="1:2" ht="63">
       <c r="A170" s="3" t="s">
         <v>327</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="31.75">
+    <row r="171" spans="1:2" ht="31.5">
       <c r="A171" s="3" t="s">
         <v>328</v>
       </c>
@@ -6270,7 +6270,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="31.75">
+    <row r="172" spans="1:2" ht="31.5">
       <c r="A172" s="3" t="s">
         <v>329</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="47.6">
+    <row r="184" spans="1:2" ht="47.25">
       <c r="A184" s="3" t="s">
         <v>319</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="31.75">
+    <row r="187" spans="1:2" ht="31.5">
       <c r="A187" s="3" t="s">
         <v>346</v>
       </c>
@@ -6406,7 +6406,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="47.6">
+    <row r="189" spans="1:2" ht="63">
       <c r="A189" s="3" t="s">
         <v>349</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="31.75">
+    <row r="190" spans="1:2" ht="31.5">
       <c r="A190" s="3" t="s">
         <v>350</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="31.75">
+    <row r="191" spans="1:2" ht="31.5">
       <c r="A191" s="3" t="s">
         <v>351</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="47.6">
+    <row r="197" spans="1:2" ht="47.25">
       <c r="A197" s="3" t="s">
         <v>361</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="47.6">
+    <row r="198" spans="1:2" ht="47.25">
       <c r="A198" s="3" t="s">
         <v>363</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="31.75">
+    <row r="201" spans="1:2" ht="31.5">
       <c r="A201" s="3" t="s">
         <v>368</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="31.75">
+    <row r="202" spans="1:2" ht="31.5">
       <c r="A202" s="3" t="s">
         <v>370</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="31.75">
+    <row r="215" spans="1:2" ht="31.5">
       <c r="A215" s="3" t="s">
         <v>395</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="47.6">
+    <row r="233" spans="1:2" ht="47.25">
       <c r="A233" s="3" t="s">
         <v>417</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="31.75">
+    <row r="235" spans="1:2" ht="31.5">
       <c r="A235" s="3" t="s">
         <v>423</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="31.75">
+    <row r="236" spans="1:2" ht="31.5">
       <c r="A236" s="3" t="s">
         <v>426</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="47.6">
+    <row r="239" spans="1:2" ht="47.25">
       <c r="A239" s="3" t="s">
         <v>435</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="47.6">
+    <row r="240" spans="1:2" ht="47.25">
       <c r="A240" s="3" t="s">
         <v>438</v>
       </c>
@@ -6822,7 +6822,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="79.3">
+    <row r="241" spans="1:2" ht="78.75">
       <c r="A241" s="3" t="s">
         <v>441</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="47.6">
+    <row r="242" spans="1:2" ht="47.25">
       <c r="A242" s="3" t="s">
         <v>444</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="79.3">
+    <row r="243" spans="1:2" ht="78.75">
       <c r="A243" s="3" t="s">
         <v>447</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="31.75">
+    <row r="244" spans="1:2" ht="31.5">
       <c r="A244" s="3" t="s">
         <v>450</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="47.6">
+    <row r="247" spans="1:2" ht="47.25">
       <c r="A247" s="3" t="s">
         <v>455</v>
       </c>
@@ -6886,7 +6886,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="31.75">
+    <row r="249" spans="1:2" ht="31.5">
       <c r="A249" s="3" t="s">
         <v>459</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="31.75">
+    <row r="250" spans="1:2" ht="31.5">
       <c r="A250" s="3" t="s">
         <v>461</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="31.75">
+    <row r="254" spans="1:2" ht="31.5">
       <c r="A254" s="3" t="s">
         <v>467</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="31.75">
+    <row r="255" spans="1:2" ht="31.5">
       <c r="A255" s="3" t="s">
         <v>469</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="31.75">
+    <row r="256" spans="1:2" ht="31.5">
       <c r="A256" s="3" t="s">
         <v>472</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="47.6">
+    <row r="257" spans="1:2" ht="47.25">
       <c r="A257" s="3" t="s">
         <v>474</v>
       </c>
@@ -6958,7 +6958,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="47.6">
+    <row r="258" spans="1:2" ht="47.25">
       <c r="A258" s="3" t="s">
         <v>477</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="63.45">
+    <row r="259" spans="1:2" ht="63">
       <c r="A259" s="3" t="s">
         <v>479</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="79.3">
+    <row r="260" spans="1:2" ht="78.75">
       <c r="A260" s="3" t="s">
         <v>481</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="79.3">
+    <row r="261" spans="1:2" ht="78.75">
       <c r="A261" s="3" t="s">
         <v>483</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="47.6">
+    <row r="262" spans="1:2" ht="47.25">
       <c r="A262" s="3" t="s">
         <v>486</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="47.6">
+    <row r="265" spans="1:2" ht="47.25">
       <c r="A265" s="3" t="s">
         <v>490</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="31.75">
+    <row r="267" spans="1:2" ht="31.5">
       <c r="A267" s="3" t="s">
         <v>492</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="31.75">
+    <row r="268" spans="1:2" ht="31.5">
       <c r="A268" s="3" t="s">
         <v>493</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="31.75">
+    <row r="272" spans="1:2" ht="31.5">
       <c r="A272" s="3" t="s">
         <v>497</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="31.75">
+    <row r="273" spans="1:2" ht="31.5">
       <c r="A273" s="3" t="s">
         <v>498</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="31.75">
+    <row r="274" spans="1:2" ht="31.5">
       <c r="A274" s="3" t="s">
         <v>499</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="47.6">
+    <row r="275" spans="1:2" ht="47.25">
       <c r="A275" s="3" t="s">
         <v>500</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="276" spans="1:2" ht="47.6">
+    <row r="276" spans="1:2" ht="47.25">
       <c r="A276" s="3" t="s">
         <v>501</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="277" spans="1:2" ht="63.45">
+    <row r="277" spans="1:2" ht="63">
       <c r="A277" s="3" t="s">
         <v>502</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="79.3">
+    <row r="278" spans="1:2" ht="78.75">
       <c r="A278" s="3" t="s">
         <v>503</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="79.3">
+    <row r="279" spans="1:2" ht="78.75">
       <c r="A279" s="3" t="s">
         <v>504</v>
       </c>
@@ -7134,7 +7134,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="280" spans="1:2" ht="47.6">
+    <row r="280" spans="1:2" ht="47.25">
       <c r="A280" s="3" t="s">
         <v>505</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="31.75">
+    <row r="283" spans="1:2" ht="31.5">
       <c r="A283" s="3" t="s">
         <v>507</v>
       </c>
@@ -7174,7 +7174,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="31.75">
+    <row r="285" spans="1:2" ht="31.5">
       <c r="A285" s="3" t="s">
         <v>511</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="47.6">
+    <row r="288" spans="1:2" ht="47.25">
       <c r="A288" s="3" t="s">
         <v>519</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="79.3">
+    <row r="291" spans="1:2" ht="78.75">
       <c r="A291" s="3" t="s">
         <v>527</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="47.6">
+    <row r="294" spans="1:2" ht="47.25">
       <c r="A294" s="3" t="s">
         <v>531</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="31.75">
+    <row r="296" spans="1:2" ht="31.5">
       <c r="A296" s="3" t="s">
         <v>533</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="31.75">
+    <row r="297" spans="1:2" ht="31.5">
       <c r="A297" s="3" t="s">
         <v>534</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="31.75">
+    <row r="301" spans="1:2" ht="31.5">
       <c r="A301" s="3" t="s">
         <v>538</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="31.75">
+    <row r="302" spans="1:2" ht="31.5">
       <c r="A302" s="3" t="s">
         <v>539</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="31.75">
+    <row r="303" spans="1:2" ht="31.5">
       <c r="A303" s="3" t="s">
         <v>540</v>
       </c>
@@ -7326,7 +7326,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="47.6">
+    <row r="304" spans="1:2" ht="47.25">
       <c r="A304" s="3" t="s">
         <v>541</v>
       </c>
@@ -7334,7 +7334,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="305" spans="1:2" ht="47.6">
+    <row r="305" spans="1:2" ht="47.25">
       <c r="A305" s="3" t="s">
         <v>542</v>
       </c>
@@ -7342,7 +7342,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="306" spans="1:2" ht="63.45">
+    <row r="306" spans="1:2" ht="63">
       <c r="A306" s="3" t="s">
         <v>543</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="307" spans="1:2" ht="79.3">
+    <row r="307" spans="1:2" ht="78.75">
       <c r="A307" s="3" t="s">
         <v>544</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="308" spans="1:2" ht="79.3">
+    <row r="308" spans="1:2" ht="78.75">
       <c r="A308" s="3" t="s">
         <v>545</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="47.6">
+    <row r="309" spans="1:2" ht="47.25">
       <c r="A309" s="3" t="s">
         <v>546</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="95.15">
+    <row r="313" spans="1:2" ht="94.5">
       <c r="A313" s="3" t="s">
         <v>548</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="31.75">
+    <row r="314" spans="1:2" ht="31.5">
       <c r="A314" s="3" t="s">
         <v>550</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="31.75">
+    <row r="320" spans="1:2" ht="31.5">
       <c r="A320" s="3" t="s">
         <v>564</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="31.75">
+    <row r="324" spans="1:2" ht="31.5">
       <c r="A324" s="3" t="s">
         <v>575</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="326" spans="1:2" ht="31.75">
+    <row r="326" spans="1:2" ht="31.5">
       <c r="A326" s="3" t="s">
         <v>581</v>
       </c>
@@ -7518,7 +7518,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="63.45">
+    <row r="328" spans="1:2" ht="63">
       <c r="A328" s="3" t="s">
         <v>587</v>
       </c>
@@ -7526,7 +7526,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="329" spans="1:2" ht="47.6">
+    <row r="329" spans="1:2" ht="47.25">
       <c r="A329" s="3" t="s">
         <v>589</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="331" spans="1:2" ht="31.75">
+    <row r="331" spans="1:2" ht="31.5">
       <c r="A331" s="3" t="s">
         <v>593</v>
       </c>
@@ -7550,7 +7550,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="332" spans="1:2" ht="31.75">
+    <row r="332" spans="1:2" ht="31.5">
       <c r="A332" s="3" t="s">
         <v>596</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="31.75">
+    <row r="339" spans="1:2" ht="31.5">
       <c r="A339" s="3" t="s">
         <v>610</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="95.15">
+    <row r="344" spans="1:2" ht="94.5">
       <c r="A344" s="3" t="s">
         <v>618</v>
       </c>
@@ -7654,7 +7654,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="31.75">
+    <row r="345" spans="1:2" ht="31.5">
       <c r="A345" s="3" t="s">
         <v>619</v>
       </c>
@@ -7702,7 +7702,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="31.75">
+    <row r="351" spans="1:2" ht="31.5">
       <c r="A351" s="3" t="s">
         <v>631</v>
       </c>
@@ -7710,7 +7710,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="31.75">
+    <row r="352" spans="1:2" ht="31.5">
       <c r="A352" s="3" t="s">
         <v>633</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="31.75">
+    <row r="353" spans="1:2" ht="31.5">
       <c r="A353" s="3" t="s">
         <v>635</v>
       </c>
@@ -7726,7 +7726,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="354" spans="1:2" ht="47.6">
+    <row r="354" spans="1:2" ht="31.5">
       <c r="A354" s="3" t="s">
         <v>637</v>
       </c>
@@ -7782,7 +7782,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="31.75">
+    <row r="361" spans="1:2" ht="31.5">
       <c r="A361" s="3" t="s">
         <v>646</v>
       </c>
@@ -7822,7 +7822,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="79.3">
+    <row r="366" spans="1:2" ht="78.75">
       <c r="A366" s="3" t="s">
         <v>650</v>
       </c>
@@ -7830,7 +7830,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="31.75">
+    <row r="367" spans="1:2" ht="31.5">
       <c r="A367" s="3" t="s">
         <v>652</v>
       </c>
@@ -7862,7 +7862,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="31.75">
+    <row r="371" spans="1:2" ht="31.5">
       <c r="A371" s="3" t="s">
         <v>658</v>
       </c>
@@ -7870,7 +7870,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="31.75">
+    <row r="372" spans="1:2" ht="31.5">
       <c r="A372" s="3" t="s">
         <v>660</v>
       </c>
@@ -7886,7 +7886,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="31.75">
+    <row r="374" spans="1:2" ht="31.5">
       <c r="A374" s="3" t="s">
         <v>665</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="31.75">
+    <row r="375" spans="1:2" ht="31.5">
       <c r="A375" s="3" t="s">
         <v>667</v>
       </c>
@@ -7902,7 +7902,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="47.6">
+    <row r="376" spans="1:2" ht="31.5">
       <c r="A376" s="3" t="s">
         <v>669</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="383" spans="1:2" ht="31.75">
+    <row r="383" spans="1:2" ht="31.5">
       <c r="A383" s="3" t="s">
         <v>676</v>
       </c>
@@ -7998,7 +7998,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="388" spans="1:2" ht="79.3">
+    <row r="388" spans="1:2" ht="78.75">
       <c r="A388" s="3" t="s">
         <v>680</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="389" spans="1:2" ht="31.75">
+    <row r="389" spans="1:2" ht="31.5">
       <c r="A389" s="3" t="s">
         <v>681</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="396" spans="1:2" ht="31.75">
+    <row r="396" spans="1:2" ht="31.5">
       <c r="A396" s="3" t="s">
         <v>691</v>
       </c>
@@ -8086,7 +8086,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="399" spans="1:2" ht="31.75">
+    <row r="399" spans="1:2" ht="31.5">
       <c r="A399" s="3" t="s">
         <v>698</v>
       </c>
@@ -8126,7 +8126,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="404" spans="1:2" ht="31.75">
+    <row r="404" spans="1:2" ht="31.5">
       <c r="A404" s="3" t="s">
         <v>707</v>
       </c>
@@ -8150,7 +8150,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="31.75">
+    <row r="407" spans="1:2" ht="31.5">
       <c r="A407" s="3" t="s">
         <v>710</v>
       </c>
@@ -8166,7 +8166,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="63.45">
+    <row r="409" spans="1:2" ht="63">
       <c r="A409" s="3" t="s">
         <v>712</v>
       </c>
@@ -8174,7 +8174,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="410" spans="1:2" ht="47.6">
+    <row r="410" spans="1:2" ht="47.25">
       <c r="A410" s="3" t="s">
         <v>713</v>
       </c>
@@ -8190,7 +8190,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="412" spans="1:2" ht="31.75">
+    <row r="412" spans="1:2" ht="31.5">
       <c r="A412" s="3" t="s">
         <v>716</v>
       </c>
@@ -8246,7 +8246,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="419" spans="1:2" ht="31.75">
+    <row r="419" spans="1:2" ht="31.5">
       <c r="A419" s="3" t="s">
         <v>723</v>
       </c>
@@ -8342,7 +8342,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="431" spans="1:2" ht="79.3">
+    <row r="431" spans="1:2" ht="78.75">
       <c r="A431" s="3" t="s">
         <v>732</v>
       </c>
@@ -8350,7 +8350,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="432" spans="1:2" ht="31.75">
+    <row r="432" spans="1:2" ht="31.5">
       <c r="A432" s="3" t="s">
         <v>733</v>
       </c>
@@ -8406,7 +8406,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="439" spans="1:2" ht="31.75">
+    <row r="439" spans="1:2" ht="31.5">
       <c r="A439" s="3" t="s">
         <v>742</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="440" spans="1:2" ht="47.6">
+    <row r="440" spans="1:2" ht="47.25">
       <c r="A440" s="3" t="s">
         <v>744</v>
       </c>
@@ -8478,7 +8478,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="448" spans="1:2" ht="31.75">
+    <row r="448" spans="1:2" ht="31.5">
       <c r="A448" s="3" t="s">
         <v>753</v>
       </c>
@@ -8517,24 +8517,24 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G472"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+    <sheetView tabSelected="1" topLeftCell="A451" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F461" sqref="F461"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.2109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.25" style="4" customWidth="1"/>
     <col min="2" max="2" width="12" style="4" customWidth="1"/>
-    <col min="3" max="3" width="43.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.75" style="4" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" style="34" customWidth="1"/>
-    <col min="6" max="6" width="84.640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="80.85546875" style="31" customWidth="1"/>
+    <col min="5" max="5" width="24.125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="84.625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="80.875" style="31" customWidth="1"/>
     <col min="8" max="1026" width="8.5" style="17" customWidth="1"/>
     <col min="1027" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="30" customFormat="1" ht="18.45">
+    <row r="1" spans="1:7" s="30" customFormat="1" ht="18.75">
       <c r="A1" s="35" t="s">
         <v>52</v>
       </c>
@@ -16604,9 +16604,7 @@
       </c>
       <c r="D449" s="40"/>
       <c r="E449" s="40"/>
-      <c r="F449" s="39" t="s">
-        <v>1183</v>
-      </c>
+      <c r="F449" s="40"/>
       <c r="G449" s="38"/>
     </row>
     <row r="450" spans="1:7">
@@ -16621,9 +16619,7 @@
       </c>
       <c r="D450" s="40"/>
       <c r="E450" s="40"/>
-      <c r="F450" s="39" t="s">
-        <v>1183</v>
-      </c>
+      <c r="F450" s="40"/>
       <c r="G450" s="40"/>
     </row>
     <row r="451" spans="1:7" ht="105">
@@ -16641,7 +16637,7 @@
       </c>
       <c r="E451" s="39"/>
       <c r="F451" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G451" s="43" t="s">
         <v>1108</v>
@@ -16662,7 +16658,7 @@
       </c>
       <c r="E452" s="39"/>
       <c r="F452" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G452" s="43"/>
     </row>
@@ -16681,7 +16677,7 @@
       </c>
       <c r="E453" s="39"/>
       <c r="F453" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G453" s="43"/>
     </row>
@@ -16697,9 +16693,7 @@
       </c>
       <c r="D454" s="40"/>
       <c r="E454" s="40"/>
-      <c r="F454" s="39" t="s">
-        <v>1183</v>
-      </c>
+      <c r="F454" s="40"/>
       <c r="G454" s="40"/>
     </row>
     <row r="455" spans="1:7">
@@ -16714,9 +16708,7 @@
       </c>
       <c r="D455" s="40"/>
       <c r="E455" s="40"/>
-      <c r="F455" s="39" t="s">
-        <v>1183</v>
-      </c>
+      <c r="F455" s="40"/>
       <c r="G455" s="40"/>
     </row>
     <row r="456" spans="1:7" ht="30">
@@ -16734,7 +16726,7 @@
       </c>
       <c r="E456" s="39"/>
       <c r="F456" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G456" s="43" t="s">
         <v>1119</v>
@@ -16755,7 +16747,7 @@
       </c>
       <c r="E457" s="39"/>
       <c r="F457" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G457" s="43"/>
     </row>
@@ -16774,7 +16766,7 @@
       </c>
       <c r="E458" s="39"/>
       <c r="F458" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G458" s="39"/>
     </row>
@@ -16793,7 +16785,7 @@
       </c>
       <c r="E459" s="39"/>
       <c r="F459" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G459" s="39"/>
     </row>
@@ -16810,7 +16802,7 @@
       <c r="D460" s="39"/>
       <c r="E460" s="39"/>
       <c r="F460" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G460" s="39"/>
     </row>
@@ -16829,7 +16821,7 @@
       </c>
       <c r="E461" s="39"/>
       <c r="F461" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G461" s="39"/>
     </row>
@@ -16848,7 +16840,7 @@
       </c>
       <c r="E462" s="39"/>
       <c r="F462" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G462" s="39"/>
     </row>
@@ -16864,9 +16856,7 @@
       </c>
       <c r="D463" s="40"/>
       <c r="E463" s="40"/>
-      <c r="F463" s="39" t="s">
-        <v>1183</v>
-      </c>
+      <c r="F463" s="40"/>
       <c r="G463" s="40"/>
     </row>
     <row r="464" spans="1:7">
@@ -16884,7 +16874,7 @@
       </c>
       <c r="E464" s="39"/>
       <c r="F464" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G464" s="43" t="s">
         <v>1111</v>
@@ -16905,7 +16895,7 @@
       </c>
       <c r="E465" s="39"/>
       <c r="F465" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G465" s="39"/>
     </row>
@@ -16921,9 +16911,7 @@
       </c>
       <c r="D466" s="40"/>
       <c r="E466" s="40"/>
-      <c r="F466" s="39" t="s">
-        <v>1183</v>
-      </c>
+      <c r="F466" s="40"/>
       <c r="G466" s="40"/>
     </row>
     <row r="467" spans="1:7">
@@ -16962,7 +16950,7 @@
       </c>
       <c r="E468" s="39"/>
       <c r="F468" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G468" s="43"/>
     </row>
@@ -16981,7 +16969,7 @@
       </c>
       <c r="E469" s="39"/>
       <c r="F469" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G469" s="43"/>
     </row>
@@ -17000,7 +16988,7 @@
       </c>
       <c r="E470" s="39"/>
       <c r="F470" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G470" s="39"/>
     </row>
@@ -17019,7 +17007,7 @@
       </c>
       <c r="E471" s="39"/>
       <c r="F471" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G471" s="39"/>
     </row>
@@ -17038,7 +17026,7 @@
       </c>
       <c r="E472" s="39"/>
       <c r="F472" s="39" t="s">
-        <v>1183</v>
+        <v>1127</v>
       </c>
       <c r="G472" s="39"/>
     </row>
@@ -17057,14 +17045,14 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.640625" style="4" customWidth="1"/>
-    <col min="4" max="5" width="81.35546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="45.125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.625" style="4" customWidth="1"/>
+    <col min="4" max="5" width="81.375" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.85546875" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.875" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -17148,7 +17136,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="126.9">
+    <row r="5" spans="1:7" ht="126">
       <c r="A5" s="3" t="s">
         <v>68</v>
       </c>
@@ -17204,15 +17192,15 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="68.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.875" style="4" customWidth="1"/>
     <col min="4" max="4" width="100" style="4" customWidth="1"/>
-    <col min="5" max="6" width="22.85546875" style="4" customWidth="1"/>
+    <col min="5" max="6" width="22.875" style="4" customWidth="1"/>
     <col min="7" max="7" width="20" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.85546875" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.875" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -17353,7 +17341,7 @@
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="31.5">
       <c r="A8" s="6" t="s">
         <v>784</v>
       </c>
@@ -17906,7 +17894,7 @@
       </c>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" ht="63.45">
+    <row r="37" spans="1:7" ht="63">
       <c r="A37" s="6" t="s">
         <v>246</v>
       </c>
@@ -17927,7 +17915,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="31.75">
+    <row r="38" spans="1:7" ht="31.5">
       <c r="A38" s="6" t="s">
         <v>509</v>
       </c>
@@ -18003,7 +17991,7 @@
       </c>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:7" ht="47.6">
+    <row r="42" spans="1:7" ht="47.25">
       <c r="A42" s="6" t="s">
         <v>263</v>
       </c>
@@ -18287,19 +18275,19 @@
       <selection sqref="A1:D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="47.35546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="4" customWidth="1"/>
-    <col min="4" max="5" width="80.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="47.375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.875" style="4" customWidth="1"/>
+    <col min="4" max="5" width="80.875" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.85546875" style="17" customWidth="1"/>
+    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.875" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="22" customFormat="1" ht="31" customHeight="1">
+    <row r="1" spans="1:256" s="22" customFormat="1" ht="30.95" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>756</v>
       </c>
@@ -18571,7 +18559,7 @@
       <c r="IU1" s="21"/>
       <c r="IV1" s="21"/>
     </row>
-    <row r="2" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="2" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>834</v>
       </c>
@@ -18590,7 +18578,7 @@
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="3" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>837</v>
       </c>
@@ -18609,7 +18597,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="4" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>839</v>
       </c>
@@ -18647,7 +18635,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="6" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>843</v>
       </c>
@@ -18666,7 +18654,7 @@
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="7" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>846</v>
       </c>
@@ -18685,7 +18673,7 @@
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="8" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>849</v>
       </c>
@@ -18723,7 +18711,7 @@
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="10" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>855</v>
       </c>
@@ -18742,7 +18730,7 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="11" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>857</v>
       </c>
@@ -18761,7 +18749,7 @@
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="12" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>859</v>
       </c>
@@ -18799,7 +18787,7 @@
       </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="14" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>864</v>
       </c>
@@ -18818,7 +18806,7 @@
       </c>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="15" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>866</v>
       </c>
@@ -18875,7 +18863,7 @@
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="18" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>868</v>
       </c>
@@ -18894,7 +18882,7 @@
       </c>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="19" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>870</v>
       </c>
@@ -18913,7 +18901,7 @@
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>872</v>
       </c>
@@ -18932,7 +18920,7 @@
       </c>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="21" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>874</v>
       </c>
@@ -18951,7 +18939,7 @@
       </c>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="22" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>877</v>
       </c>
@@ -18970,7 +18958,7 @@
       </c>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="23" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>879</v>
       </c>
@@ -18989,7 +18977,7 @@
       </c>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="24" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>881</v>
       </c>
@@ -19008,7 +18996,7 @@
       </c>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="25" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>883</v>
       </c>
@@ -19027,7 +19015,7 @@
       </c>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="26" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>886</v>
       </c>
@@ -19046,7 +19034,7 @@
       </c>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="27" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>888</v>
       </c>
@@ -19065,7 +19053,7 @@
       </c>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="28" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>891</v>
       </c>
@@ -19084,7 +19072,7 @@
       </c>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="29" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>893</v>
       </c>
@@ -19103,7 +19091,7 @@
       </c>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="30" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>895</v>
       </c>
@@ -19122,7 +19110,7 @@
       </c>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="31" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>897</v>
       </c>
@@ -19141,7 +19129,7 @@
       </c>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="32" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>900</v>
       </c>
@@ -19160,7 +19148,7 @@
       </c>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="33" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>903</v>
       </c>
@@ -19179,7 +19167,7 @@
       </c>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="34" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A34" s="6" t="s">
         <v>906</v>
       </c>
@@ -19198,7 +19186,7 @@
       </c>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="35" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A35" s="6" t="s">
         <v>909</v>
       </c>
@@ -19217,7 +19205,7 @@
       </c>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="36" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A36" s="6" t="s">
         <v>912</v>
       </c>
@@ -19236,7 +19224,7 @@
       </c>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="37" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>915</v>
       </c>
@@ -19255,7 +19243,7 @@
       </c>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="38" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A38" s="6" t="s">
         <v>918</v>
       </c>
@@ -19274,7 +19262,7 @@
       </c>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="39" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A39" s="6" t="s">
         <v>921</v>
       </c>
@@ -19293,7 +19281,7 @@
       </c>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" ht="31" customHeight="1">
+    <row r="40" spans="1:7" ht="30.95" customHeight="1">
       <c r="A40" s="6" t="s">
         <v>924</v>
       </c>
@@ -19329,7 +19317,7 @@
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="42" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A42" s="6" t="s">
         <v>931</v>
       </c>
@@ -19346,7 +19334,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:7" ht="31" customHeight="1">
+    <row r="43" spans="1:7" ht="30.95" customHeight="1">
       <c r="A43" s="6" t="s">
         <v>934</v>
       </c>
@@ -19384,7 +19372,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="45" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A45" s="6" t="s">
         <v>942</v>
       </c>
@@ -19437,7 +19425,7 @@
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="48" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A48" s="6" t="s">
         <v>952</v>
       </c>
@@ -19454,7 +19442,7 @@
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:256" s="29" customFormat="1" ht="31.75">
+    <row r="49" spans="1:256" s="29" customFormat="1" ht="31.5">
       <c r="A49" s="53" t="s">
         <v>955</v>
       </c>
@@ -19750,21 +19738,21 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="33.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="44.35546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="41.35546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="44.375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41.375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="4" customWidth="1"/>
     <col min="7" max="7" width="29" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.85546875" style="17" customWidth="1"/>
+    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.875" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.149999999999999" customHeight="1">
+    <row r="1" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="53" t="s">
         <v>756</v>
       </c>
@@ -20230,7 +20218,7 @@
       <c r="F24" s="66"/>
       <c r="G24" s="66"/>
     </row>
-    <row r="25" spans="1:7" ht="43.75">
+    <row r="25" spans="1:7" ht="45">
       <c r="A25" s="66" t="s">
         <v>1211</v>
       </c>
@@ -20247,7 +20235,7 @@
       <c r="F25" s="66"/>
       <c r="G25" s="66"/>
     </row>
-    <row r="26" spans="1:7" ht="29.15">
+    <row r="26" spans="1:7" ht="30">
       <c r="A26" s="66" t="s">
         <v>1260</v>
       </c>
@@ -20264,7 +20252,7 @@
       <c r="F26" s="66"/>
       <c r="G26" s="66"/>
     </row>
-    <row r="27" spans="1:7" ht="29.15">
+    <row r="27" spans="1:7" ht="30">
       <c r="A27" s="66" t="s">
         <v>1263</v>
       </c>
@@ -20281,7 +20269,7 @@
       <c r="F27" s="66"/>
       <c r="G27" s="66"/>
     </row>
-    <row r="28" spans="1:7" ht="29.15">
+    <row r="28" spans="1:7" ht="30">
       <c r="A28" s="66" t="s">
         <v>1266</v>
       </c>
@@ -20298,7 +20286,7 @@
       <c r="F28" s="66"/>
       <c r="G28" s="66"/>
     </row>
-    <row r="29" spans="1:7" ht="29.15">
+    <row r="29" spans="1:7" ht="30">
       <c r="A29" s="66" t="s">
         <v>1269</v>
       </c>
@@ -20315,7 +20303,7 @@
       <c r="F29" s="66"/>
       <c r="G29" s="66"/>
     </row>
-    <row r="30" spans="1:7" ht="29.15">
+    <row r="30" spans="1:7" ht="30">
       <c r="A30" s="66" t="s">
         <v>1272</v>
       </c>
@@ -20350,15 +20338,15 @@
       <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="54.640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="4" customWidth="1"/>
-    <col min="4" max="5" width="75.640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="54.625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.875" style="4" customWidth="1"/>
+    <col min="4" max="5" width="75.625" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.85546875" style="17" customWidth="1"/>
+    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.875" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
@@ -20423,7 +20411,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="63.45">
+    <row r="4" spans="1:7" ht="63">
       <c r="A4" s="5" t="s">
         <v>1004</v>
       </c>
@@ -20456,23 +20444,25 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="53.35546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="53.375" style="18" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="18" customWidth="1"/>
     <col min="4" max="4" width="44.5" style="18" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" style="18" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="31.875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="11.875" style="18" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="18" customWidth="1"/>
-    <col min="8" max="256" width="8.85546875" style="18" customWidth="1"/>
-    <col min="257" max="1025" width="8.85546875" style="19" customWidth="1"/>
+    <col min="8" max="256" width="8.875" style="18" customWidth="1"/>
+    <col min="257" max="1025" width="8.875" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="25" customFormat="1" ht="17.149999999999999" customHeight="1">
+    <row r="1" spans="1:256" s="25" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>756</v>
       </c>
@@ -20763,7 +20753,7 @@
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="3" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>627</v>
       </c>
@@ -20782,7 +20772,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="4" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>557</v>
       </c>
@@ -20801,7 +20791,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="5" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>560</v>
       </c>
@@ -20820,7 +20810,7 @@
       </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="6" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>563</v>
       </c>
@@ -20839,7 +20829,7 @@
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:256" ht="301.3">
+    <row r="7" spans="1:256" ht="315">
       <c r="A7" s="6" t="s">
         <v>566</v>
       </c>
@@ -20862,7 +20852,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="8" spans="1:256" ht="31.75">
+    <row r="8" spans="1:256" ht="31.5">
       <c r="A8" s="6" t="s">
         <v>571</v>
       </c>
@@ -20919,7 +20909,7 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="11" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>580</v>
       </c>
@@ -20938,7 +20928,7 @@
       </c>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:256" ht="33.65" customHeight="1">
+    <row r="12" spans="1:256" ht="33.6" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>583</v>
       </c>
@@ -21100,7 +21090,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="20" spans="1:256" ht="17.149999999999999" customHeight="1">
+    <row r="20" spans="1:256" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>697</v>
       </c>
@@ -21165,7 +21155,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="23" spans="1:256" s="33" customFormat="1" ht="31.75">
+    <row r="23" spans="1:256" s="33" customFormat="1" ht="31.5">
       <c r="A23" s="6" t="s">
         <v>1071</v>
       </c>
@@ -21965,7 +21955,7 @@
       <c r="IU25" s="32"/>
       <c r="IV25" s="32"/>
     </row>
-    <row r="26" spans="1:256" s="33" customFormat="1" ht="31.75">
+    <row r="26" spans="1:256" s="33" customFormat="1" ht="31.5">
       <c r="A26" s="6" t="s">
         <v>1067</v>
       </c>
@@ -22513,19 +22503,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.5" style="20" customWidth="1"/>
-    <col min="2" max="2" width="53.35546875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="53.375" style="17" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="17" customWidth="1"/>
     <col min="4" max="5" width="44.5" style="17" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="11.875" style="17" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="17" customWidth="1"/>
-    <col min="8" max="1025" width="8.85546875" style="17" customWidth="1"/>
+    <col min="8" max="1025" width="8.875" style="17" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="22" customFormat="1" ht="17.149999999999999" customHeight="1">
+    <row r="1" spans="1:256" s="22" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="51" t="s">
         <v>756</v>
       </c>
@@ -22797,7 +22787,7 @@
       <c r="IU1" s="21"/>
       <c r="IV1" s="21"/>
     </row>
-    <row r="2" spans="1:256" ht="31.75">
+    <row r="2" spans="1:256" ht="31.5">
       <c r="A2" s="52" t="s">
         <v>1200</v>
       </c>
@@ -22818,7 +22808,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="31.75">
+    <row r="3" spans="1:256" ht="31.5">
       <c r="A3" s="52" t="s">
         <v>1284</v>
       </c>
@@ -22839,7 +22829,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:256" ht="31.75">
+    <row r="4" spans="1:256" ht="31.5">
       <c r="A4" s="6" t="s">
         <v>1287</v>
       </c>

</xml_diff>

<commit_message>
Fixed Carillon-specific content signing policy OID
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV-I_Carillon.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV-I_Carillon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9391F86A-6016-4C3F-8BB4-7AEE3AB495D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0060DA00-D169-4D53-986B-96BFAF41BE5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="1815" windowWidth="26190" windowHeight="13845" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="1815" windowWidth="26190" windowHeight="13845" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -3958,13 +3958,13 @@
     <t>These policies would only work for directly-asserted OIDs.  PIV-I are normally mapped.  Use the Override feature to configure PCI OIDs.</t>
   </si>
   <si>
+    <t>1.3.6.1.4.1.45606.3.1.22</t>
+  </si>
+  <si>
     <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,
 X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,
 X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,
-CARD_HOLDER_UNIQUE_IDENTIFIER_OID;1.3.6.1.4.1.45606.3.1.22</t>
-  </si>
-  <si>
-    <t>1.3.6.1.4.1.45606.3.1.22</t>
+CARD_HOLDER_UNIQUE_IDENTIFIER_OID;1.3.6.1.4.1.45606.3.1.21</t>
   </si>
 </sst>
 </file>
@@ -8517,8 +8517,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A451" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F461" sqref="F461"/>
+    <sheetView topLeftCell="A379" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D377" sqref="D377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -20444,7 +20444,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -20843,7 +20843,7 @@
         <v>1019</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>764</v>
@@ -21146,7 +21146,7 @@
         <v>1053</v>
       </c>
       <c r="E22" s="68" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>783</v>

</xml_diff>

<commit_message>
Cleaned up test cases
Fixed container OID for content signing cert
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV-I_Carillon.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV-I_Carillon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0060DA00-D169-4D53-986B-96BFAF41BE5E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A215E1DA-ADD6-4D07-B807-6B4B3EF59A59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="1815" windowWidth="26190" windowHeight="13845" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4320" yWindow="2505" windowWidth="16485" windowHeight="13845" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3769" uniqueCount="1309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="1309">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3964,7 +3964,7 @@
     <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,
 X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,
 X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,
-CARD_HOLDER_UNIQUE_IDENTIFIER_OID;1.3.6.1.4.1.45606.3.1.21</t>
+CARD_HOLDER_UNIQUE_IDENTIFIER_OID;1.3.6.1.4.1.45606.3.1.22</t>
   </si>
 </sst>
 </file>
@@ -8515,10 +8515,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G472"/>
+  <dimension ref="A1:G471"/>
   <sheetViews>
-    <sheetView topLeftCell="A379" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D377" sqref="D377"/>
+    <sheetView tabSelected="1" topLeftCell="A340" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A349" sqref="A349:XFD349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -14718,18 +14718,18 @@
       </c>
       <c r="G348" s="43"/>
     </row>
-    <row r="349" spans="1:7">
+    <row r="349" spans="1:7" ht="45">
       <c r="A349" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B349" s="39" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="C349" s="43" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="D349" s="39" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="E349" s="39"/>
       <c r="F349" s="39" t="s">
@@ -14737,49 +14737,51 @@
       </c>
       <c r="G349" s="43"/>
     </row>
-    <row r="350" spans="1:7" ht="45">
+    <row r="350" spans="1:7">
       <c r="A350" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B350" s="39" t="s">
-        <v>581</v>
-      </c>
-      <c r="C350" s="43" t="s">
-        <v>582</v>
-      </c>
-      <c r="D350" s="39" t="s">
-        <v>583</v>
-      </c>
-      <c r="E350" s="39"/>
-      <c r="F350" s="39" t="s">
+        <v>584</v>
+      </c>
+      <c r="C350" s="40" t="s">
+        <v>585</v>
+      </c>
+      <c r="D350" s="40"/>
+      <c r="E350" s="40"/>
+      <c r="F350" s="40"/>
+      <c r="G350" s="40"/>
+    </row>
+    <row r="351" spans="1:7" ht="90">
+      <c r="A351" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B351" s="39" t="s">
+        <v>587</v>
+      </c>
+      <c r="C351" s="43" t="s">
+        <v>588</v>
+      </c>
+      <c r="D351" s="39" t="s">
+        <v>586</v>
+      </c>
+      <c r="E351" s="39"/>
+      <c r="F351" s="39" t="s">
         <v>1159</v>
       </c>
-      <c r="G350" s="43"/>
-    </row>
-    <row r="351" spans="1:7">
-      <c r="A351" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B351" s="39" t="s">
-        <v>584</v>
-      </c>
-      <c r="C351" s="40" t="s">
-        <v>585</v>
-      </c>
-      <c r="D351" s="40"/>
-      <c r="E351" s="40"/>
-      <c r="F351" s="40"/>
-      <c r="G351" s="40"/>
-    </row>
-    <row r="352" spans="1:7" ht="90">
+      <c r="G351" s="43" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" ht="60">
       <c r="A352" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B352" s="39" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="C352" s="43" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="D352" s="39" t="s">
         <v>586</v>
@@ -14788,60 +14790,58 @@
       <c r="F352" s="39" t="s">
         <v>1159</v>
       </c>
-      <c r="G352" s="43" t="s">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="353" spans="1:7" ht="60">
+      <c r="G352" s="43"/>
+    </row>
+    <row r="353" spans="1:7" ht="30">
       <c r="A353" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B353" s="39" t="s">
-        <v>589</v>
-      </c>
-      <c r="C353" s="43" t="s">
-        <v>590</v>
+        <v>591</v>
+      </c>
+      <c r="C353" s="39" t="s">
+        <v>592</v>
       </c>
       <c r="D353" s="39" t="s">
-        <v>586</v>
+        <v>1200</v>
       </c>
       <c r="E353" s="39"/>
       <c r="F353" s="39" t="s">
         <v>1159</v>
       </c>
-      <c r="G353" s="43"/>
-    </row>
-    <row r="354" spans="1:7" ht="30">
+      <c r="G353" s="39"/>
+    </row>
+    <row r="354" spans="1:7" ht="45">
       <c r="A354" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B354" s="39" t="s">
-        <v>591</v>
-      </c>
-      <c r="C354" s="39" t="s">
-        <v>592</v>
+        <v>593</v>
+      </c>
+      <c r="C354" s="43" t="s">
+        <v>594</v>
       </c>
       <c r="D354" s="39" t="s">
-        <v>1200</v>
+        <v>595</v>
       </c>
       <c r="E354" s="39"/>
       <c r="F354" s="39" t="s">
         <v>1159</v>
       </c>
-      <c r="G354" s="39"/>
-    </row>
-    <row r="355" spans="1:7" ht="45">
+      <c r="G354" s="43"/>
+    </row>
+    <row r="355" spans="1:7" ht="30">
       <c r="A355" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B355" s="39" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="C355" s="43" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="D355" s="39" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="E355" s="39"/>
       <c r="F355" s="39" t="s">
@@ -14849,147 +14849,147 @@
       </c>
       <c r="G355" s="43"/>
     </row>
-    <row r="356" spans="1:7" ht="30">
+    <row r="356" spans="1:7">
       <c r="A356" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B356" s="39" t="s">
-        <v>596</v>
-      </c>
-      <c r="C356" s="43" t="s">
-        <v>597</v>
-      </c>
-      <c r="D356" s="39" t="s">
-        <v>598</v>
-      </c>
-      <c r="E356" s="39"/>
-      <c r="F356" s="39" t="s">
-        <v>1159</v>
-      </c>
-      <c r="G356" s="43"/>
+        <v>599</v>
+      </c>
+      <c r="C356" s="40" t="s">
+        <v>600</v>
+      </c>
+      <c r="D356" s="40"/>
+      <c r="E356" s="40"/>
+      <c r="F356" s="40"/>
+      <c r="G356" s="40"/>
     </row>
     <row r="357" spans="1:7">
       <c r="A357" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B357" s="39" t="s">
-        <v>599</v>
-      </c>
-      <c r="C357" s="40" t="s">
-        <v>600</v>
-      </c>
-      <c r="D357" s="40"/>
-      <c r="E357" s="40"/>
-      <c r="F357" s="40"/>
-      <c r="G357" s="40"/>
+        <v>601</v>
+      </c>
+      <c r="C357" s="43" t="s">
+        <v>602</v>
+      </c>
+      <c r="D357" s="39" t="s">
+        <v>577</v>
+      </c>
+      <c r="E357" s="39"/>
+      <c r="F357" s="39" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G357" s="39" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="358" spans="1:7">
       <c r="A358" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B358" s="39" t="s">
-        <v>601</v>
-      </c>
-      <c r="C358" s="43" t="s">
-        <v>602</v>
+        <v>603</v>
+      </c>
+      <c r="C358" s="39" t="s">
+        <v>604</v>
       </c>
       <c r="D358" s="39" t="s">
-        <v>577</v>
+        <v>1066</v>
       </c>
       <c r="E358" s="39"/>
       <c r="F358" s="39" t="s">
         <v>1159</v>
       </c>
-      <c r="G358" s="39" t="s">
-        <v>1111</v>
-      </c>
+      <c r="G358" s="39"/>
     </row>
     <row r="359" spans="1:7">
       <c r="A359" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B359" s="39" t="s">
-        <v>603</v>
-      </c>
-      <c r="C359" s="39" t="s">
-        <v>604</v>
-      </c>
-      <c r="D359" s="39" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E359" s="39"/>
-      <c r="F359" s="39" t="s">
-        <v>1159</v>
-      </c>
-      <c r="G359" s="39"/>
+        <v>605</v>
+      </c>
+      <c r="C359" s="40" t="s">
+        <v>606</v>
+      </c>
+      <c r="D359" s="40"/>
+      <c r="E359" s="40"/>
+      <c r="F359" s="40"/>
+      <c r="G359" s="40"/>
     </row>
     <row r="360" spans="1:7">
       <c r="A360" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B360" s="39" t="s">
-        <v>605</v>
-      </c>
-      <c r="C360" s="40" t="s">
-        <v>606</v>
-      </c>
-      <c r="D360" s="40"/>
-      <c r="E360" s="40"/>
-      <c r="F360" s="40"/>
-      <c r="G360" s="40"/>
-    </row>
-    <row r="361" spans="1:7">
+        <v>607</v>
+      </c>
+      <c r="C360" s="43" t="s">
+        <v>570</v>
+      </c>
+      <c r="D360" s="39" t="s">
+        <v>571</v>
+      </c>
+      <c r="E360" s="39"/>
+      <c r="F360" s="39" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G360" s="43" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" ht="30">
       <c r="A361" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B361" s="39" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C361" s="43" t="s">
-        <v>570</v>
+        <v>609</v>
       </c>
       <c r="D361" s="39" t="s">
-        <v>571</v>
-      </c>
-      <c r="E361" s="39"/>
+        <v>1071</v>
+      </c>
+      <c r="E361" s="46"/>
       <c r="F361" s="39" t="s">
         <v>1159</v>
       </c>
-      <c r="G361" s="43" t="s">
-        <v>1112</v>
-      </c>
+      <c r="G361" s="43"/>
     </row>
     <row r="362" spans="1:7" ht="30">
       <c r="A362" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B362" s="39" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="C362" s="43" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="D362" s="39" t="s">
-        <v>1071</v>
-      </c>
-      <c r="E362" s="46"/>
+        <v>577</v>
+      </c>
+      <c r="E362" s="39"/>
       <c r="F362" s="39" t="s">
         <v>1159</v>
       </c>
       <c r="G362" s="43"/>
     </row>
-    <row r="363" spans="1:7" ht="30">
+    <row r="363" spans="1:7">
       <c r="A363" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B363" s="39" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C363" s="43" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="D363" s="39" t="s">
-        <v>577</v>
+        <v>1069</v>
       </c>
       <c r="E363" s="39"/>
       <c r="F363" s="39" t="s">
@@ -14997,150 +14997,146 @@
       </c>
       <c r="G363" s="43"/>
     </row>
-    <row r="364" spans="1:7">
+    <row r="364" spans="1:7" ht="30">
       <c r="A364" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B364" s="39" t="s">
-        <v>612</v>
-      </c>
-      <c r="C364" s="43" t="s">
-        <v>613</v>
+        <v>614</v>
+      </c>
+      <c r="C364" s="39" t="s">
+        <v>615</v>
       </c>
       <c r="D364" s="39" t="s">
-        <v>1069</v>
-      </c>
-      <c r="E364" s="39"/>
+        <v>1067</v>
+      </c>
+      <c r="E364" s="39" t="s">
+        <v>616</v>
+      </c>
       <c r="F364" s="39" t="s">
         <v>1159</v>
       </c>
-      <c r="G364" s="43"/>
-    </row>
-    <row r="365" spans="1:7" ht="30">
+      <c r="G364" s="39"/>
+    </row>
+    <row r="365" spans="1:7">
       <c r="A365" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B365" s="39" t="s">
-        <v>614</v>
-      </c>
-      <c r="C365" s="39" t="s">
-        <v>615</v>
-      </c>
-      <c r="D365" s="39" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E365" s="39" t="s">
-        <v>616</v>
-      </c>
-      <c r="F365" s="39" t="s">
-        <v>1159</v>
-      </c>
-      <c r="G365" s="39"/>
+      <c r="B365" s="39">
+        <v>11.2</v>
+      </c>
+      <c r="C365" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D365" s="40"/>
+      <c r="E365" s="40"/>
+      <c r="F365" s="40"/>
+      <c r="G365" s="40"/>
     </row>
     <row r="366" spans="1:7">
       <c r="A366" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B366" s="39">
-        <v>11.2</v>
-      </c>
-      <c r="C366" s="38" t="s">
-        <v>44</v>
+      <c r="B366" s="39" t="s">
+        <v>617</v>
+      </c>
+      <c r="C366" s="40" t="s">
+        <v>42</v>
       </c>
       <c r="D366" s="40"/>
       <c r="E366" s="40"/>
       <c r="F366" s="40"/>
       <c r="G366" s="40"/>
     </row>
-    <row r="367" spans="1:7">
+    <row r="367" spans="1:7" ht="120">
       <c r="A367" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B367" s="39" t="s">
-        <v>617</v>
-      </c>
-      <c r="C367" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D367" s="40"/>
-      <c r="E367" s="40"/>
-      <c r="F367" s="40"/>
-      <c r="G367" s="40"/>
-    </row>
-    <row r="368" spans="1:7" ht="120">
+        <v>618</v>
+      </c>
+      <c r="C367" s="43" t="s">
+        <v>549</v>
+      </c>
+      <c r="D367" s="39" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E367" s="39" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F367" s="39" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G367" s="43" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" ht="75">
       <c r="A368" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B368" s="39" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C368" s="43" t="s">
-        <v>549</v>
+        <v>620</v>
       </c>
       <c r="D368" s="39" t="s">
-        <v>1004</v>
+        <v>999</v>
       </c>
       <c r="E368" s="39" t="s">
-        <v>1207</v>
+        <v>1221</v>
       </c>
       <c r="F368" s="39" t="s">
         <v>1177</v>
       </c>
-      <c r="G368" s="43" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="369" spans="1:7" ht="75">
+      <c r="G368" s="43"/>
+    </row>
+    <row r="369" spans="1:7" ht="30">
       <c r="A369" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B369" s="39" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C369" s="43" t="s">
-        <v>620</v>
-      </c>
-      <c r="D369" s="39" t="s">
-        <v>999</v>
+        <v>553</v>
+      </c>
+      <c r="D369" s="39">
+        <v>78.099999999999994</v>
       </c>
       <c r="E369" s="39" t="s">
-        <v>1221</v>
+        <v>1207</v>
       </c>
       <c r="F369" s="39" t="s">
         <v>1177</v>
       </c>
       <c r="G369" s="43"/>
     </row>
-    <row r="370" spans="1:7" ht="30">
+    <row r="370" spans="1:7">
       <c r="A370" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B370" s="39" t="s">
-        <v>621</v>
-      </c>
-      <c r="C370" s="43" t="s">
-        <v>553</v>
-      </c>
-      <c r="D370" s="39">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E370" s="39" t="s">
-        <v>1207</v>
-      </c>
-      <c r="F370" s="39" t="s">
-        <v>1177</v>
-      </c>
-      <c r="G370" s="43"/>
+        <v>622</v>
+      </c>
+      <c r="C370" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D370" s="40"/>
+      <c r="E370" s="40"/>
+      <c r="F370" s="40"/>
+      <c r="G370" s="40"/>
     </row>
     <row r="371" spans="1:7">
       <c r="A371" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B371" s="39" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C371" s="40" t="s">
-        <v>43</v>
+        <v>624</v>
       </c>
       <c r="D371" s="40"/>
       <c r="E371" s="40"/>
@@ -15152,49 +15148,53 @@
         <v>56</v>
       </c>
       <c r="B372" s="39" t="s">
-        <v>623</v>
-      </c>
-      <c r="C372" s="40" t="s">
-        <v>624</v>
-      </c>
-      <c r="D372" s="40"/>
-      <c r="E372" s="40"/>
-      <c r="F372" s="40"/>
-      <c r="G372" s="40"/>
-    </row>
-    <row r="373" spans="1:7">
+        <v>625</v>
+      </c>
+      <c r="C372" s="39" t="s">
+        <v>626</v>
+      </c>
+      <c r="D372" s="39" t="s">
+        <v>627</v>
+      </c>
+      <c r="E372" s="39"/>
+      <c r="F372" s="39" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G372" s="43" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" ht="30">
       <c r="A373" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B373" s="39" t="s">
-        <v>625</v>
-      </c>
-      <c r="C373" s="39" t="s">
-        <v>626</v>
+        <v>628</v>
+      </c>
+      <c r="C373" s="43" t="s">
+        <v>629</v>
       </c>
       <c r="D373" s="39" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="E373" s="39"/>
       <c r="F373" s="39" t="s">
         <v>1177</v>
       </c>
-      <c r="G373" s="43" t="s">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="374" spans="1:7" ht="30">
+      <c r="G373" s="43"/>
+    </row>
+    <row r="374" spans="1:7" ht="45">
       <c r="A374" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B374" s="39" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="C374" s="43" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="D374" s="39" t="s">
-        <v>630</v>
+        <v>583</v>
       </c>
       <c r="E374" s="39"/>
       <c r="F374" s="39" t="s">
@@ -15207,13 +15207,13 @@
         <v>56</v>
       </c>
       <c r="B375" s="39" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="C375" s="43" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="D375" s="39" t="s">
-        <v>583</v>
+        <v>595</v>
       </c>
       <c r="E375" s="39"/>
       <c r="F375" s="39" t="s">
@@ -15221,18 +15221,18 @@
       </c>
       <c r="G375" s="43"/>
     </row>
-    <row r="376" spans="1:7" ht="45">
+    <row r="376" spans="1:7" ht="30">
       <c r="A376" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B376" s="39" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="C376" s="43" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="D376" s="39" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="E376" s="39"/>
       <c r="F376" s="39" t="s">
@@ -15240,18 +15240,18 @@
       </c>
       <c r="G376" s="43"/>
     </row>
-    <row r="377" spans="1:7" ht="30">
+    <row r="377" spans="1:7" ht="45">
       <c r="A377" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B377" s="39" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="C377" s="43" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="D377" s="39" t="s">
-        <v>598</v>
+        <v>566</v>
       </c>
       <c r="E377" s="39"/>
       <c r="F377" s="39" t="s">
@@ -15259,354 +15259,354 @@
       </c>
       <c r="G377" s="43"/>
     </row>
-    <row r="378" spans="1:7" ht="45">
+    <row r="378" spans="1:7">
       <c r="A378" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B378" s="39" t="s">
-        <v>637</v>
-      </c>
-      <c r="C378" s="43" t="s">
-        <v>638</v>
-      </c>
-      <c r="D378" s="39" t="s">
-        <v>566</v>
-      </c>
-      <c r="E378" s="39"/>
-      <c r="F378" s="39" t="s">
-        <v>1177</v>
-      </c>
-      <c r="G378" s="43"/>
+        <v>639</v>
+      </c>
+      <c r="C378" s="40" t="s">
+        <v>600</v>
+      </c>
+      <c r="D378" s="40"/>
+      <c r="E378" s="40"/>
+      <c r="F378" s="40"/>
+      <c r="G378" s="40"/>
     </row>
     <row r="379" spans="1:7">
       <c r="A379" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B379" s="39" t="s">
-        <v>639</v>
-      </c>
-      <c r="C379" s="40" t="s">
-        <v>600</v>
-      </c>
-      <c r="D379" s="40"/>
-      <c r="E379" s="40"/>
-      <c r="F379" s="40"/>
-      <c r="G379" s="40"/>
+        <v>640</v>
+      </c>
+      <c r="C379" s="43" t="s">
+        <v>602</v>
+      </c>
+      <c r="D379" s="39" t="s">
+        <v>577</v>
+      </c>
+      <c r="E379" s="39"/>
+      <c r="F379" s="39" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G379" s="43" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="380" spans="1:7">
       <c r="A380" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B380" s="39" t="s">
-        <v>640</v>
-      </c>
-      <c r="C380" s="43" t="s">
-        <v>602</v>
+        <v>641</v>
+      </c>
+      <c r="C380" s="39" t="s">
+        <v>604</v>
       </c>
       <c r="D380" s="39" t="s">
-        <v>577</v>
-      </c>
-      <c r="E380" s="39"/>
+        <v>1066</v>
+      </c>
+      <c r="E380" s="39" t="s">
+        <v>1222</v>
+      </c>
       <c r="F380" s="39" t="s">
         <v>1177</v>
       </c>
-      <c r="G380" s="43" t="s">
-        <v>1111</v>
-      </c>
+      <c r="G380" s="39"/>
     </row>
     <row r="381" spans="1:7">
       <c r="A381" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B381" s="39" t="s">
-        <v>641</v>
-      </c>
-      <c r="C381" s="39" t="s">
-        <v>604</v>
-      </c>
-      <c r="D381" s="39" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E381" s="39" t="s">
-        <v>1222</v>
-      </c>
-      <c r="F381" s="39" t="s">
-        <v>1177</v>
-      </c>
-      <c r="G381" s="39"/>
+        <v>642</v>
+      </c>
+      <c r="C381" s="40" t="s">
+        <v>606</v>
+      </c>
+      <c r="D381" s="40"/>
+      <c r="E381" s="40"/>
+      <c r="F381" s="40"/>
+      <c r="G381" s="40"/>
     </row>
     <row r="382" spans="1:7">
       <c r="A382" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B382" s="39" t="s">
-        <v>642</v>
-      </c>
-      <c r="C382" s="40" t="s">
-        <v>606</v>
-      </c>
-      <c r="D382" s="40"/>
-      <c r="E382" s="40"/>
-      <c r="F382" s="40"/>
-      <c r="G382" s="40"/>
-    </row>
-    <row r="383" spans="1:7">
+        <v>643</v>
+      </c>
+      <c r="C382" s="43" t="s">
+        <v>570</v>
+      </c>
+      <c r="D382" s="39" t="s">
+        <v>571</v>
+      </c>
+      <c r="E382" s="39"/>
+      <c r="F382" s="39" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G382" s="43" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" ht="30">
       <c r="A383" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B383" s="39" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C383" s="43" t="s">
-        <v>570</v>
+        <v>645</v>
       </c>
       <c r="D383" s="39" t="s">
-        <v>571</v>
-      </c>
-      <c r="E383" s="39"/>
+        <v>1071</v>
+      </c>
+      <c r="E383" s="46"/>
       <c r="F383" s="39" t="s">
         <v>1177</v>
       </c>
-      <c r="G383" s="43" t="s">
-        <v>1112</v>
-      </c>
+      <c r="G383" s="43"/>
     </row>
     <row r="384" spans="1:7" ht="30">
       <c r="A384" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B384" s="39" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="C384" s="43" t="s">
-        <v>645</v>
+        <v>611</v>
       </c>
       <c r="D384" s="39" t="s">
-        <v>1071</v>
-      </c>
-      <c r="E384" s="46"/>
+        <v>577</v>
+      </c>
+      <c r="E384" s="39"/>
       <c r="F384" s="39" t="s">
         <v>1177</v>
       </c>
       <c r="G384" s="43"/>
     </row>
-    <row r="385" spans="1:7" ht="30">
+    <row r="385" spans="1:7">
       <c r="A385" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B385" s="39" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C385" s="43" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="D385" s="39" t="s">
-        <v>577</v>
+        <v>1069</v>
       </c>
       <c r="E385" s="39"/>
       <c r="F385" s="39" t="s">
         <v>1177</v>
       </c>
-      <c r="G385" s="43"/>
-    </row>
-    <row r="386" spans="1:7">
+      <c r="G385" s="39"/>
+    </row>
+    <row r="386" spans="1:7" ht="30">
       <c r="A386" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B386" s="39" t="s">
-        <v>647</v>
-      </c>
-      <c r="C386" s="43" t="s">
-        <v>613</v>
+        <v>648</v>
+      </c>
+      <c r="C386" s="39" t="s">
+        <v>615</v>
       </c>
       <c r="D386" s="39" t="s">
-        <v>1069</v>
-      </c>
-      <c r="E386" s="39"/>
+        <v>1067</v>
+      </c>
+      <c r="E386" s="39" t="s">
+        <v>616</v>
+      </c>
       <c r="F386" s="39" t="s">
         <v>1177</v>
       </c>
       <c r="G386" s="39"/>
     </row>
-    <row r="387" spans="1:7" ht="30">
+    <row r="387" spans="1:7">
       <c r="A387" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B387" s="39" t="s">
-        <v>648</v>
-      </c>
-      <c r="C387" s="39" t="s">
-        <v>615</v>
-      </c>
-      <c r="D387" s="39" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E387" s="39" t="s">
-        <v>616</v>
-      </c>
-      <c r="F387" s="39" t="s">
-        <v>1177</v>
-      </c>
-      <c r="G387" s="39"/>
+      <c r="B387" s="39">
+        <v>11.3</v>
+      </c>
+      <c r="C387" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="D387" s="40"/>
+      <c r="E387" s="40"/>
+      <c r="F387" s="40"/>
+      <c r="G387" s="40"/>
     </row>
     <row r="388" spans="1:7">
       <c r="A388" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B388" s="39">
-        <v>11.3</v>
-      </c>
-      <c r="C388" s="38" t="s">
-        <v>45</v>
+      <c r="B388" s="39" t="s">
+        <v>649</v>
+      </c>
+      <c r="C388" s="40" t="s">
+        <v>42</v>
       </c>
       <c r="D388" s="40"/>
       <c r="E388" s="40"/>
       <c r="F388" s="40"/>
       <c r="G388" s="40"/>
     </row>
-    <row r="389" spans="1:7">
+    <row r="389" spans="1:7" ht="105">
       <c r="A389" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B389" s="39" t="s">
-        <v>649</v>
-      </c>
-      <c r="C389" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D389" s="40"/>
-      <c r="E389" s="40"/>
-      <c r="F389" s="40"/>
-      <c r="G389" s="40"/>
-    </row>
-    <row r="390" spans="1:7" ht="105">
+        <v>650</v>
+      </c>
+      <c r="C389" s="43" t="s">
+        <v>651</v>
+      </c>
+      <c r="D389" s="39">
+        <v>78.3</v>
+      </c>
+      <c r="E389" s="39" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F389" s="39" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G389" s="43" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" ht="60">
       <c r="A390" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B390" s="39" t="s">
-        <v>650</v>
-      </c>
-      <c r="C390" s="43" t="s">
-        <v>651</v>
-      </c>
-      <c r="D390" s="39">
-        <v>78.3</v>
+        <v>652</v>
+      </c>
+      <c r="C390" s="39" t="s">
+        <v>653</v>
+      </c>
+      <c r="D390" s="39" t="s">
+        <v>999</v>
       </c>
       <c r="E390" s="39" t="s">
-        <v>1207</v>
+        <v>1223</v>
       </c>
       <c r="F390" s="39" t="s">
         <v>1180</v>
       </c>
-      <c r="G390" s="43" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="391" spans="1:7" ht="60">
+      <c r="G390" s="39"/>
+    </row>
+    <row r="391" spans="1:7" ht="30">
       <c r="A391" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B391" s="39" t="s">
-        <v>652</v>
-      </c>
-      <c r="C391" s="39" t="s">
-        <v>653</v>
-      </c>
-      <c r="D391" s="39" t="s">
-        <v>999</v>
+        <v>654</v>
+      </c>
+      <c r="C391" s="43" t="s">
+        <v>655</v>
+      </c>
+      <c r="D391" s="39">
+        <v>78.099999999999994</v>
       </c>
       <c r="E391" s="39" t="s">
-        <v>1223</v>
+        <v>1207</v>
       </c>
       <c r="F391" s="39" t="s">
         <v>1180</v>
       </c>
-      <c r="G391" s="39"/>
-    </row>
-    <row r="392" spans="1:7" ht="30">
+      <c r="G391" s="43"/>
+    </row>
+    <row r="392" spans="1:7">
       <c r="A392" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B392" s="39" t="s">
-        <v>654</v>
-      </c>
-      <c r="C392" s="43" t="s">
-        <v>655</v>
-      </c>
-      <c r="D392" s="39">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E392" s="39" t="s">
-        <v>1207</v>
-      </c>
-      <c r="F392" s="39" t="s">
-        <v>1180</v>
-      </c>
-      <c r="G392" s="43"/>
+        <v>656</v>
+      </c>
+      <c r="C392" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D392" s="40"/>
+      <c r="E392" s="40"/>
+      <c r="F392" s="40"/>
+      <c r="G392" s="40"/>
     </row>
     <row r="393" spans="1:7">
       <c r="A393" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B393" s="39" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="C393" s="40" t="s">
-        <v>43</v>
+        <v>624</v>
       </c>
       <c r="D393" s="40"/>
       <c r="E393" s="40"/>
       <c r="F393" s="40"/>
       <c r="G393" s="40"/>
     </row>
-    <row r="394" spans="1:7">
+    <row r="394" spans="1:7" ht="45">
       <c r="A394" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B394" s="39" t="s">
-        <v>657</v>
-      </c>
-      <c r="C394" s="40" t="s">
-        <v>624</v>
-      </c>
-      <c r="D394" s="40"/>
-      <c r="E394" s="40"/>
-      <c r="F394" s="40"/>
-      <c r="G394" s="40"/>
+        <v>658</v>
+      </c>
+      <c r="C394" s="43" t="s">
+        <v>659</v>
+      </c>
+      <c r="D394" s="39" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E394" s="39"/>
+      <c r="F394" s="39" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G394" s="43" t="s">
+        <v>1114</v>
+      </c>
     </row>
     <row r="395" spans="1:7" ht="45">
       <c r="A395" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B395" s="39" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="C395" s="43" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="D395" s="39" t="s">
-        <v>1037</v>
+        <v>662</v>
       </c>
       <c r="E395" s="39"/>
       <c r="F395" s="39" t="s">
         <v>1180</v>
       </c>
-      <c r="G395" s="43" t="s">
-        <v>1114</v>
-      </c>
-    </row>
-    <row r="396" spans="1:7" ht="45">
+      <c r="G395" s="43"/>
+    </row>
+    <row r="396" spans="1:7">
       <c r="A396" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B396" s="39" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="C396" s="43" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="D396" s="39" t="s">
-        <v>662</v>
+        <v>560</v>
       </c>
       <c r="E396" s="39"/>
       <c r="F396" s="39" t="s">
@@ -15614,18 +15614,18 @@
       </c>
       <c r="G396" s="43"/>
     </row>
-    <row r="397" spans="1:7">
+    <row r="397" spans="1:7" ht="45">
       <c r="A397" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B397" s="39" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="C397" s="43" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="D397" s="39" t="s">
-        <v>560</v>
+        <v>583</v>
       </c>
       <c r="E397" s="39"/>
       <c r="F397" s="39" t="s">
@@ -15633,18 +15633,18 @@
       </c>
       <c r="G397" s="43"/>
     </row>
-    <row r="398" spans="1:7" ht="45">
+    <row r="398" spans="1:7" ht="30">
       <c r="A398" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B398" s="39" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="C398" s="43" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="D398" s="39" t="s">
-        <v>583</v>
+        <v>598</v>
       </c>
       <c r="E398" s="39"/>
       <c r="F398" s="39" t="s">
@@ -15652,18 +15652,18 @@
       </c>
       <c r="G398" s="43"/>
     </row>
-    <row r="399" spans="1:7" ht="30">
+    <row r="399" spans="1:7" ht="45">
       <c r="A399" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B399" s="39" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="C399" s="43" t="s">
-        <v>668</v>
+        <v>638</v>
       </c>
       <c r="D399" s="39" t="s">
-        <v>598</v>
+        <v>566</v>
       </c>
       <c r="E399" s="39"/>
       <c r="F399" s="39" t="s">
@@ -15671,300 +15671,296 @@
       </c>
       <c r="G399" s="43"/>
     </row>
-    <row r="400" spans="1:7" ht="45">
+    <row r="400" spans="1:7">
       <c r="A400" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B400" s="39" t="s">
-        <v>669</v>
-      </c>
-      <c r="C400" s="43" t="s">
-        <v>638</v>
-      </c>
-      <c r="D400" s="39" t="s">
-        <v>566</v>
-      </c>
-      <c r="E400" s="39"/>
-      <c r="F400" s="39" t="s">
-        <v>1180</v>
-      </c>
-      <c r="G400" s="43"/>
+        <v>670</v>
+      </c>
+      <c r="C400" s="40" t="s">
+        <v>600</v>
+      </c>
+      <c r="D400" s="40"/>
+      <c r="E400" s="40"/>
+      <c r="F400" s="40"/>
+      <c r="G400" s="40"/>
     </row>
     <row r="401" spans="1:7">
       <c r="A401" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B401" s="39" t="s">
-        <v>670</v>
-      </c>
-      <c r="C401" s="40" t="s">
-        <v>600</v>
-      </c>
-      <c r="D401" s="40"/>
-      <c r="E401" s="40"/>
-      <c r="F401" s="40"/>
-      <c r="G401" s="40"/>
+        <v>671</v>
+      </c>
+      <c r="C401" s="43" t="s">
+        <v>602</v>
+      </c>
+      <c r="D401" s="39" t="s">
+        <v>577</v>
+      </c>
+      <c r="E401" s="39"/>
+      <c r="F401" s="39" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G401" s="43" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="402" spans="1:7">
       <c r="A402" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B402" s="39" t="s">
-        <v>671</v>
-      </c>
-      <c r="C402" s="43" t="s">
-        <v>602</v>
+        <v>672</v>
+      </c>
+      <c r="C402" s="39" t="s">
+        <v>604</v>
       </c>
       <c r="D402" s="39" t="s">
-        <v>577</v>
-      </c>
-      <c r="E402" s="39"/>
+        <v>1066</v>
+      </c>
+      <c r="E402" s="39" t="s">
+        <v>1222</v>
+      </c>
       <c r="F402" s="39" t="s">
         <v>1180</v>
       </c>
-      <c r="G402" s="43" t="s">
-        <v>1111</v>
-      </c>
+      <c r="G402" s="39"/>
     </row>
     <row r="403" spans="1:7">
       <c r="A403" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B403" s="39" t="s">
-        <v>672</v>
-      </c>
-      <c r="C403" s="39" t="s">
-        <v>604</v>
-      </c>
-      <c r="D403" s="39" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E403" s="39" t="s">
-        <v>1222</v>
-      </c>
-      <c r="F403" s="39" t="s">
-        <v>1180</v>
-      </c>
-      <c r="G403" s="39"/>
+        <v>673</v>
+      </c>
+      <c r="C403" s="40" t="s">
+        <v>606</v>
+      </c>
+      <c r="D403" s="40"/>
+      <c r="E403" s="40"/>
+      <c r="F403" s="40"/>
+      <c r="G403" s="40"/>
     </row>
     <row r="404" spans="1:7">
       <c r="A404" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B404" s="39" t="s">
-        <v>673</v>
-      </c>
-      <c r="C404" s="40" t="s">
-        <v>606</v>
-      </c>
-      <c r="D404" s="40"/>
-      <c r="E404" s="40"/>
-      <c r="F404" s="40"/>
-      <c r="G404" s="40"/>
-    </row>
-    <row r="405" spans="1:7">
+        <v>674</v>
+      </c>
+      <c r="C404" s="43" t="s">
+        <v>570</v>
+      </c>
+      <c r="D404" s="39" t="s">
+        <v>571</v>
+      </c>
+      <c r="E404" s="39"/>
+      <c r="F404" s="39" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G404" s="43" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" ht="30">
       <c r="A405" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B405" s="39" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="C405" s="43" t="s">
-        <v>570</v>
+        <v>645</v>
       </c>
       <c r="D405" s="39" t="s">
-        <v>571</v>
-      </c>
-      <c r="E405" s="39"/>
+        <v>1071</v>
+      </c>
+      <c r="E405" s="46"/>
       <c r="F405" s="39" t="s">
         <v>1180</v>
       </c>
-      <c r="G405" s="43" t="s">
-        <v>1112</v>
-      </c>
+      <c r="G405" s="43"/>
     </row>
     <row r="406" spans="1:7" ht="30">
       <c r="A406" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B406" s="39" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="C406" s="43" t="s">
-        <v>645</v>
+        <v>611</v>
       </c>
       <c r="D406" s="39" t="s">
-        <v>1071</v>
-      </c>
-      <c r="E406" s="46"/>
+        <v>577</v>
+      </c>
+      <c r="E406" s="39"/>
       <c r="F406" s="39" t="s">
         <v>1180</v>
       </c>
       <c r="G406" s="43"/>
     </row>
-    <row r="407" spans="1:7" ht="30">
+    <row r="407" spans="1:7">
       <c r="A407" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B407" s="39" t="s">
-        <v>676</v>
-      </c>
-      <c r="C407" s="43" t="s">
-        <v>611</v>
+        <v>677</v>
+      </c>
+      <c r="C407" s="39" t="s">
+        <v>613</v>
       </c>
       <c r="D407" s="39" t="s">
-        <v>577</v>
+        <v>1069</v>
       </c>
       <c r="E407" s="39"/>
       <c r="F407" s="39" t="s">
         <v>1180</v>
       </c>
-      <c r="G407" s="43"/>
-    </row>
-    <row r="408" spans="1:7">
+      <c r="G407" s="39"/>
+    </row>
+    <row r="408" spans="1:7" ht="30">
       <c r="A408" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B408" s="39" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="C408" s="39" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D408" s="39" t="s">
-        <v>1069</v>
-      </c>
-      <c r="E408" s="39"/>
+        <v>1067</v>
+      </c>
+      <c r="E408" s="39" t="s">
+        <v>616</v>
+      </c>
       <c r="F408" s="39" t="s">
         <v>1180</v>
       </c>
       <c r="G408" s="39"/>
     </row>
-    <row r="409" spans="1:7" ht="30">
+    <row r="409" spans="1:7">
       <c r="A409" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B409" s="39" t="s">
-        <v>678</v>
-      </c>
-      <c r="C409" s="39" t="s">
-        <v>615</v>
-      </c>
-      <c r="D409" s="39" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E409" s="39" t="s">
-        <v>616</v>
-      </c>
-      <c r="F409" s="39" t="s">
-        <v>1180</v>
-      </c>
-      <c r="G409" s="39"/>
+      <c r="B409" s="39">
+        <v>11.4</v>
+      </c>
+      <c r="C409" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D409" s="40"/>
+      <c r="E409" s="40"/>
+      <c r="F409" s="40"/>
+      <c r="G409" s="40"/>
     </row>
     <row r="410" spans="1:7">
       <c r="A410" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B410" s="39">
-        <v>11.4</v>
-      </c>
-      <c r="C410" s="38" t="s">
-        <v>46</v>
+      <c r="B410" s="39" t="s">
+        <v>679</v>
+      </c>
+      <c r="C410" s="40" t="s">
+        <v>42</v>
       </c>
       <c r="D410" s="40"/>
       <c r="E410" s="40"/>
       <c r="F410" s="40"/>
       <c r="G410" s="40"/>
     </row>
-    <row r="411" spans="1:7">
+    <row r="411" spans="1:7" ht="105">
       <c r="A411" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B411" s="39" t="s">
-        <v>679</v>
-      </c>
-      <c r="C411" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D411" s="40"/>
-      <c r="E411" s="40"/>
-      <c r="F411" s="40"/>
-      <c r="G411" s="40"/>
-    </row>
-    <row r="412" spans="1:7" ht="105">
+        <v>680</v>
+      </c>
+      <c r="C411" s="43" t="s">
+        <v>651</v>
+      </c>
+      <c r="D411" s="39">
+        <v>78.3</v>
+      </c>
+      <c r="E411" s="6" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F411" s="39" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G411" s="43" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" ht="90">
       <c r="A412" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B412" s="39" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C412" s="43" t="s">
-        <v>651</v>
+        <v>682</v>
       </c>
       <c r="D412" s="39">
-        <v>78.3</v>
-      </c>
-      <c r="E412" s="6" t="s">
-        <v>1224</v>
+        <v>78.099999999999994</v>
+      </c>
+      <c r="E412" s="39" t="s">
+        <v>1225</v>
       </c>
       <c r="F412" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G412" s="43" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="413" spans="1:7" ht="90">
+      <c r="G412" s="43"/>
+    </row>
+    <row r="413" spans="1:7" ht="30">
       <c r="A413" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B413" s="39" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="C413" s="43" t="s">
-        <v>682</v>
+        <v>655</v>
       </c>
       <c r="D413" s="39">
         <v>78.099999999999994</v>
       </c>
       <c r="E413" s="39" t="s">
-        <v>1225</v>
+        <v>1207</v>
       </c>
       <c r="F413" s="39" t="s">
         <v>1183</v>
       </c>
       <c r="G413" s="43"/>
     </row>
-    <row r="414" spans="1:7" ht="30">
+    <row r="414" spans="1:7">
       <c r="A414" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B414" s="39" t="s">
-        <v>683</v>
-      </c>
-      <c r="C414" s="43" t="s">
-        <v>655</v>
-      </c>
-      <c r="D414" s="39">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E414" s="39" t="s">
-        <v>1207</v>
-      </c>
-      <c r="F414" s="39" t="s">
-        <v>1183</v>
-      </c>
-      <c r="G414" s="43"/>
+        <v>684</v>
+      </c>
+      <c r="C414" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D414" s="40"/>
+      <c r="E414" s="40"/>
+      <c r="F414" s="40"/>
+      <c r="G414" s="40"/>
     </row>
     <row r="415" spans="1:7">
       <c r="A415" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B415" s="39" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="C415" s="40" t="s">
-        <v>43</v>
+        <v>624</v>
       </c>
       <c r="D415" s="40"/>
       <c r="E415" s="40"/>
@@ -15976,49 +15972,53 @@
         <v>56</v>
       </c>
       <c r="B416" s="39" t="s">
-        <v>685</v>
-      </c>
-      <c r="C416" s="40" t="s">
-        <v>624</v>
-      </c>
-      <c r="D416" s="40"/>
-      <c r="E416" s="40"/>
-      <c r="F416" s="40"/>
-      <c r="G416" s="40"/>
+        <v>686</v>
+      </c>
+      <c r="C416" s="39" t="s">
+        <v>626</v>
+      </c>
+      <c r="D416" s="39" t="s">
+        <v>627</v>
+      </c>
+      <c r="E416" s="39"/>
+      <c r="F416" s="39" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G416" s="39" t="s">
+        <v>1115</v>
+      </c>
     </row>
     <row r="417" spans="1:7">
       <c r="A417" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B417" s="39" t="s">
-        <v>686</v>
-      </c>
-      <c r="C417" s="39" t="s">
-        <v>626</v>
+        <v>687</v>
+      </c>
+      <c r="C417" s="43" t="s">
+        <v>688</v>
       </c>
       <c r="D417" s="39" t="s">
-        <v>627</v>
+        <v>557</v>
       </c>
       <c r="E417" s="39"/>
       <c r="F417" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G417" s="39" t="s">
-        <v>1115</v>
-      </c>
+      <c r="G417" s="43"/>
     </row>
     <row r="418" spans="1:7">
       <c r="A418" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B418" s="39" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="C418" s="43" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="D418" s="39" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="E418" s="39"/>
       <c r="F418" s="39" t="s">
@@ -16026,89 +16026,89 @@
       </c>
       <c r="G418" s="43"/>
     </row>
-    <row r="419" spans="1:7">
+    <row r="419" spans="1:7" ht="30">
       <c r="A419" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B419" s="39" t="s">
-        <v>689</v>
-      </c>
-      <c r="C419" s="43" t="s">
-        <v>690</v>
+        <v>691</v>
+      </c>
+      <c r="C419" s="39" t="s">
+        <v>692</v>
       </c>
       <c r="D419" s="39" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="E419" s="39"/>
       <c r="F419" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G419" s="43"/>
-    </row>
-    <row r="420" spans="1:7" ht="30">
+      <c r="G419" s="39"/>
+    </row>
+    <row r="420" spans="1:7">
       <c r="A420" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B420" s="39" t="s">
-        <v>691</v>
-      </c>
-      <c r="C420" s="39" t="s">
-        <v>692</v>
-      </c>
-      <c r="D420" s="39" t="s">
-        <v>566</v>
-      </c>
-      <c r="E420" s="39"/>
-      <c r="F420" s="39" t="s">
+        <v>693</v>
+      </c>
+      <c r="C420" s="40" t="s">
+        <v>694</v>
+      </c>
+      <c r="D420" s="40"/>
+      <c r="E420" s="40"/>
+      <c r="F420" s="40"/>
+      <c r="G420" s="40"/>
+    </row>
+    <row r="421" spans="1:7" ht="30">
+      <c r="A421" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B421" s="39" t="s">
+        <v>695</v>
+      </c>
+      <c r="C421" s="39" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D421" s="39" t="s">
+        <v>697</v>
+      </c>
+      <c r="E421" s="39"/>
+      <c r="F421" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G420" s="39"/>
-    </row>
-    <row r="421" spans="1:7">
-      <c r="A421" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B421" s="39" t="s">
-        <v>693</v>
-      </c>
-      <c r="C421" s="40" t="s">
-        <v>694</v>
-      </c>
-      <c r="D421" s="40"/>
-      <c r="E421" s="40"/>
-      <c r="F421" s="40"/>
-      <c r="G421" s="40"/>
+      <c r="G421" s="39" t="s">
+        <v>1116</v>
+      </c>
     </row>
     <row r="422" spans="1:7" ht="30">
       <c r="A422" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B422" s="39" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="C422" s="39" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
       <c r="D422" s="39" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="E422" s="39"/>
       <c r="F422" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G422" s="39" t="s">
-        <v>1116</v>
-      </c>
+      <c r="G422" s="39"/>
     </row>
     <row r="423" spans="1:7" ht="30">
       <c r="A423" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B423" s="39" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="C423" s="39" t="s">
-        <v>1291</v>
+        <v>702</v>
       </c>
       <c r="D423" s="39" t="s">
         <v>700</v>
@@ -16119,73 +16119,73 @@
       </c>
       <c r="G423" s="39"/>
     </row>
-    <row r="424" spans="1:7" ht="30">
+    <row r="424" spans="1:7">
       <c r="A424" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B424" s="39" t="s">
-        <v>701</v>
-      </c>
-      <c r="C424" s="39" t="s">
-        <v>702</v>
-      </c>
-      <c r="D424" s="39" t="s">
-        <v>700</v>
-      </c>
-      <c r="E424" s="39"/>
-      <c r="F424" s="39" t="s">
-        <v>1183</v>
-      </c>
-      <c r="G424" s="39"/>
+        <v>703</v>
+      </c>
+      <c r="C424" s="40" t="s">
+        <v>606</v>
+      </c>
+      <c r="D424" s="40"/>
+      <c r="E424" s="40"/>
+      <c r="F424" s="40"/>
+      <c r="G424" s="40"/>
     </row>
     <row r="425" spans="1:7">
       <c r="A425" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B425" s="39" t="s">
-        <v>703</v>
-      </c>
-      <c r="C425" s="40" t="s">
-        <v>606</v>
-      </c>
-      <c r="D425" s="40"/>
-      <c r="E425" s="40"/>
-      <c r="F425" s="40"/>
-      <c r="G425" s="40"/>
+        <v>704</v>
+      </c>
+      <c r="C425" s="43" t="s">
+        <v>570</v>
+      </c>
+      <c r="D425" s="39" t="s">
+        <v>571</v>
+      </c>
+      <c r="E425" s="39"/>
+      <c r="F425" s="39" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G425" s="43" t="s">
+        <v>1117</v>
+      </c>
     </row>
     <row r="426" spans="1:7">
       <c r="A426" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B426" s="39" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C426" s="43" t="s">
-        <v>570</v>
+        <v>706</v>
       </c>
       <c r="D426" s="39" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="E426" s="39"/>
       <c r="F426" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G426" s="43" t="s">
-        <v>1117</v>
-      </c>
-    </row>
-    <row r="427" spans="1:7">
+      <c r="G426" s="43"/>
+    </row>
+    <row r="427" spans="1:7" ht="30">
       <c r="A427" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B427" s="39" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="C427" s="43" t="s">
-        <v>706</v>
+        <v>611</v>
       </c>
       <c r="D427" s="39" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="E427" s="39"/>
       <c r="F427" s="39" t="s">
@@ -16193,15 +16193,15 @@
       </c>
       <c r="G427" s="43"/>
     </row>
-    <row r="428" spans="1:7" ht="30">
+    <row r="428" spans="1:7">
       <c r="A428" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B428" s="39" t="s">
-        <v>707</v>
-      </c>
-      <c r="C428" s="43" t="s">
-        <v>611</v>
+        <v>708</v>
+      </c>
+      <c r="C428" s="39" t="s">
+        <v>613</v>
       </c>
       <c r="D428" s="39" t="s">
         <v>577</v>
@@ -16210,39 +16210,39 @@
       <c r="F428" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G428" s="43"/>
+      <c r="G428" s="39"/>
     </row>
     <row r="429" spans="1:7">
       <c r="A429" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B429" s="39" t="s">
-        <v>708</v>
-      </c>
-      <c r="C429" s="39" t="s">
-        <v>613</v>
+        <v>709</v>
+      </c>
+      <c r="C429" s="43" t="s">
+        <v>579</v>
       </c>
       <c r="D429" s="39" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="E429" s="39"/>
       <c r="F429" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G429" s="39"/>
-    </row>
-    <row r="430" spans="1:7">
+      <c r="G429" s="43"/>
+    </row>
+    <row r="430" spans="1:7" ht="45">
       <c r="A430" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B430" s="39" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C430" s="43" t="s">
-        <v>579</v>
+        <v>666</v>
       </c>
       <c r="D430" s="39" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="E430" s="39"/>
       <c r="F430" s="39" t="s">
@@ -16250,51 +16250,53 @@
       </c>
       <c r="G430" s="43"/>
     </row>
-    <row r="431" spans="1:7" ht="45">
+    <row r="431" spans="1:7">
       <c r="A431" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B431" s="39" t="s">
-        <v>710</v>
-      </c>
-      <c r="C431" s="43" t="s">
-        <v>666</v>
-      </c>
-      <c r="D431" s="39" t="s">
-        <v>583</v>
-      </c>
-      <c r="E431" s="39"/>
+        <v>711</v>
+      </c>
+      <c r="C431" s="40" t="s">
+        <v>585</v>
+      </c>
+      <c r="D431" s="40"/>
+      <c r="E431" s="40"/>
       <c r="F431" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G431" s="43"/>
-    </row>
-    <row r="432" spans="1:7">
+      <c r="G431" s="40"/>
+    </row>
+    <row r="432" spans="1:7" ht="90">
       <c r="A432" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B432" s="39" t="s">
-        <v>711</v>
-      </c>
-      <c r="C432" s="40" t="s">
-        <v>585</v>
-      </c>
-      <c r="D432" s="40"/>
-      <c r="E432" s="40"/>
+        <v>712</v>
+      </c>
+      <c r="C432" s="43" t="s">
+        <v>588</v>
+      </c>
+      <c r="D432" s="39" t="s">
+        <v>586</v>
+      </c>
+      <c r="E432" s="39"/>
       <c r="F432" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G432" s="40"/>
-    </row>
-    <row r="433" spans="1:7" ht="90">
+      <c r="G432" s="43" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="433" spans="1:7" ht="60">
       <c r="A433" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B433" s="39" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C433" s="43" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="D433" s="39" t="s">
         <v>586</v>
@@ -16303,19 +16305,17 @@
       <c r="F433" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G433" s="43" t="s">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="434" spans="1:7" ht="60">
+      <c r="G433" s="43"/>
+    </row>
+    <row r="434" spans="1:7" ht="30">
       <c r="A434" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B434" s="39" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C434" s="43" t="s">
-        <v>590</v>
+        <v>715</v>
       </c>
       <c r="D434" s="39" t="s">
         <v>586</v>
@@ -16324,171 +16324,171 @@
       <c r="F434" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G434" s="43"/>
+      <c r="G434" s="43" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="435" spans="1:7" ht="30">
       <c r="A435" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B435" s="39" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="C435" s="43" t="s">
-        <v>715</v>
+        <v>668</v>
       </c>
       <c r="D435" s="39" t="s">
-        <v>586</v>
+        <v>598</v>
       </c>
       <c r="E435" s="39"/>
       <c r="F435" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G435" s="43" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="436" spans="1:7" ht="30">
+      <c r="G435" s="43"/>
+    </row>
+    <row r="436" spans="1:7">
       <c r="A436" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B436" s="39" t="s">
-        <v>716</v>
-      </c>
-      <c r="C436" s="43" t="s">
-        <v>668</v>
-      </c>
-      <c r="D436" s="39" t="s">
-        <v>598</v>
-      </c>
-      <c r="E436" s="39"/>
+        <v>717</v>
+      </c>
+      <c r="C436" s="40" t="s">
+        <v>600</v>
+      </c>
+      <c r="D436" s="40"/>
+      <c r="E436" s="40"/>
       <c r="F436" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G436" s="43"/>
+      <c r="G436" s="40"/>
     </row>
     <row r="437" spans="1:7">
       <c r="A437" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B437" s="39" t="s">
-        <v>717</v>
-      </c>
-      <c r="C437" s="40" t="s">
-        <v>600</v>
-      </c>
-      <c r="D437" s="40"/>
-      <c r="E437" s="40"/>
+        <v>718</v>
+      </c>
+      <c r="C437" s="43" t="s">
+        <v>602</v>
+      </c>
+      <c r="D437" s="39" t="s">
+        <v>577</v>
+      </c>
+      <c r="E437" s="39"/>
       <c r="F437" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G437" s="40"/>
+      <c r="G437" s="43" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="438" spans="1:7">
       <c r="A438" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B438" s="39" t="s">
-        <v>718</v>
-      </c>
-      <c r="C438" s="43" t="s">
-        <v>602</v>
+        <v>719</v>
+      </c>
+      <c r="C438" s="39" t="s">
+        <v>604</v>
       </c>
       <c r="D438" s="39" t="s">
-        <v>577</v>
-      </c>
-      <c r="E438" s="39"/>
+        <v>1066</v>
+      </c>
+      <c r="E438" s="39" t="s">
+        <v>1222</v>
+      </c>
       <c r="F438" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G438" s="43" t="s">
-        <v>1111</v>
-      </c>
+      <c r="G438" s="39"/>
     </row>
     <row r="439" spans="1:7">
       <c r="A439" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B439" s="39" t="s">
-        <v>719</v>
-      </c>
-      <c r="C439" s="39" t="s">
-        <v>604</v>
-      </c>
-      <c r="D439" s="39" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E439" s="39" t="s">
-        <v>1222</v>
-      </c>
+        <v>720</v>
+      </c>
+      <c r="C439" s="40" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D439" s="40"/>
+      <c r="E439" s="40"/>
       <c r="F439" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G439" s="39"/>
-    </row>
-    <row r="440" spans="1:7">
+      <c r="G439" s="40"/>
+    </row>
+    <row r="440" spans="1:7" ht="30">
       <c r="A440" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B440" s="39" t="s">
-        <v>720</v>
-      </c>
-      <c r="C440" s="40" t="s">
-        <v>1076</v>
-      </c>
-      <c r="D440" s="40"/>
-      <c r="E440" s="40"/>
+        <v>725</v>
+      </c>
+      <c r="C440" s="39" t="s">
+        <v>615</v>
+      </c>
+      <c r="D440" s="39" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E440" s="39" t="s">
+        <v>616</v>
+      </c>
       <c r="F440" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G440" s="40"/>
-    </row>
-    <row r="441" spans="1:7" ht="30">
+      <c r="G440" s="39"/>
+    </row>
+    <row r="441" spans="1:7">
       <c r="A441" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B441" s="39" t="s">
-        <v>725</v>
-      </c>
-      <c r="C441" s="39" t="s">
-        <v>615</v>
-      </c>
-      <c r="D441" s="39" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E441" s="39" t="s">
-        <v>616</v>
-      </c>
+      <c r="B441" s="39">
+        <v>11.5</v>
+      </c>
+      <c r="C441" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D441" s="40"/>
+      <c r="E441" s="40"/>
       <c r="F441" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G441" s="39"/>
+      <c r="G441" s="38"/>
     </row>
     <row r="442" spans="1:7">
       <c r="A442" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B442" s="39">
-        <v>11.5</v>
-      </c>
-      <c r="C442" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D442" s="40"/>
-      <c r="E442" s="40"/>
+      <c r="B442" s="39" t="s">
+        <v>726</v>
+      </c>
+      <c r="C442" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D442" s="39"/>
+      <c r="E442" s="43" t="s">
+        <v>268</v>
+      </c>
       <c r="F442" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G442" s="38"/>
+      <c r="G442" s="43"/>
     </row>
     <row r="443" spans="1:7">
       <c r="A443" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B443" s="39" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C443" s="43" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D443" s="39"/>
       <c r="E443" s="43" t="s">
@@ -16504,10 +16504,10 @@
         <v>56</v>
       </c>
       <c r="B444" s="39" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C444" s="43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D444" s="39"/>
       <c r="E444" s="43" t="s">
@@ -16522,47 +16522,47 @@
       <c r="A445" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B445" s="39" t="s">
-        <v>728</v>
-      </c>
-      <c r="C445" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D445" s="39"/>
-      <c r="E445" s="43" t="s">
-        <v>268</v>
-      </c>
+      <c r="B445" s="39">
+        <v>11.6</v>
+      </c>
+      <c r="C445" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D445" s="40"/>
+      <c r="E445" s="38"/>
       <c r="F445" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G445" s="43"/>
+      <c r="G445" s="38"/>
     </row>
     <row r="446" spans="1:7">
       <c r="A446" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B446" s="39">
-        <v>11.6</v>
-      </c>
-      <c r="C446" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="D446" s="40"/>
-      <c r="E446" s="38"/>
+      <c r="B446" s="39" t="s">
+        <v>729</v>
+      </c>
+      <c r="C446" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D446" s="39"/>
+      <c r="E446" s="43" t="s">
+        <v>268</v>
+      </c>
       <c r="F446" s="39" t="s">
         <v>1183</v>
       </c>
-      <c r="G446" s="38"/>
+      <c r="G446" s="43"/>
     </row>
     <row r="447" spans="1:7">
       <c r="A447" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B447" s="39" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C447" s="43" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D447" s="39"/>
       <c r="E447" s="43" t="s">
@@ -16577,81 +16577,81 @@
       <c r="A448" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B448" s="39" t="s">
-        <v>730</v>
-      </c>
-      <c r="C448" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="D448" s="39"/>
-      <c r="E448" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="F448" s="39" t="s">
-        <v>1183</v>
-      </c>
-      <c r="G448" s="43"/>
+      <c r="B448" s="39">
+        <v>11.7</v>
+      </c>
+      <c r="C448" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D448" s="40"/>
+      <c r="E448" s="40"/>
+      <c r="F448" s="40"/>
+      <c r="G448" s="38"/>
     </row>
     <row r="449" spans="1:7">
       <c r="A449" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B449" s="39">
-        <v>11.7</v>
-      </c>
-      <c r="C449" s="38" t="s">
-        <v>51</v>
+      <c r="B449" s="39" t="s">
+        <v>731</v>
+      </c>
+      <c r="C449" s="40" t="s">
+        <v>42</v>
       </c>
       <c r="D449" s="40"/>
       <c r="E449" s="40"/>
       <c r="F449" s="40"/>
-      <c r="G449" s="38"/>
-    </row>
-    <row r="450" spans="1:7">
+      <c r="G449" s="40"/>
+    </row>
+    <row r="450" spans="1:7" ht="105">
       <c r="A450" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B450" s="39" t="s">
-        <v>731</v>
-      </c>
-      <c r="C450" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D450" s="40"/>
-      <c r="E450" s="40"/>
-      <c r="F450" s="40"/>
-      <c r="G450" s="40"/>
-    </row>
-    <row r="451" spans="1:7" ht="105">
+        <v>732</v>
+      </c>
+      <c r="C450" s="43" t="s">
+        <v>651</v>
+      </c>
+      <c r="D450" s="39">
+        <v>78.3</v>
+      </c>
+      <c r="E450" s="39"/>
+      <c r="F450" s="39" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G450" s="43" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="451" spans="1:7" ht="30">
       <c r="A451" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B451" s="39" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C451" s="43" t="s">
-        <v>651</v>
+        <v>682</v>
       </c>
       <c r="D451" s="39">
-        <v>78.3</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="E451" s="39"/>
       <c r="F451" s="39" t="s">
         <v>1127</v>
       </c>
-      <c r="G451" s="43" t="s">
-        <v>1108</v>
-      </c>
+      <c r="G451" s="43"/>
     </row>
     <row r="452" spans="1:7" ht="30">
       <c r="A452" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B452" s="39" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="C452" s="43" t="s">
-        <v>682</v>
+        <v>655</v>
       </c>
       <c r="D452" s="39">
         <v>78.099999999999994</v>
@@ -16662,107 +16662,107 @@
       </c>
       <c r="G452" s="43"/>
     </row>
-    <row r="453" spans="1:7" ht="30">
+    <row r="453" spans="1:7">
       <c r="A453" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B453" s="39" t="s">
-        <v>734</v>
-      </c>
-      <c r="C453" s="43" t="s">
-        <v>655</v>
-      </c>
-      <c r="D453" s="39">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E453" s="39"/>
-      <c r="F453" s="39" t="s">
-        <v>1127</v>
-      </c>
-      <c r="G453" s="43"/>
+        <v>735</v>
+      </c>
+      <c r="C453" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D453" s="40"/>
+      <c r="E453" s="40"/>
+      <c r="F453" s="40"/>
+      <c r="G453" s="40"/>
     </row>
     <row r="454" spans="1:7">
       <c r="A454" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B454" s="39" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C454" s="40" t="s">
-        <v>43</v>
+        <v>624</v>
       </c>
       <c r="D454" s="40"/>
       <c r="E454" s="40"/>
       <c r="F454" s="40"/>
       <c r="G454" s="40"/>
     </row>
-    <row r="455" spans="1:7">
+    <row r="455" spans="1:7" ht="30">
       <c r="A455" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B455" s="39" t="s">
-        <v>736</v>
-      </c>
-      <c r="C455" s="40" t="s">
-        <v>624</v>
-      </c>
-      <c r="D455" s="40"/>
-      <c r="E455" s="40"/>
-      <c r="F455" s="40"/>
-      <c r="G455" s="40"/>
-    </row>
-    <row r="456" spans="1:7" ht="30">
+        <v>737</v>
+      </c>
+      <c r="C455" s="43" t="s">
+        <v>738</v>
+      </c>
+      <c r="D455" s="39" t="s">
+        <v>557</v>
+      </c>
+      <c r="E455" s="39"/>
+      <c r="F455" s="39" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G455" s="43" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="456" spans="1:7">
       <c r="A456" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B456" s="39" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C456" s="43" t="s">
-        <v>738</v>
+        <v>690</v>
       </c>
       <c r="D456" s="39" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="E456" s="39"/>
       <c r="F456" s="39" t="s">
         <v>1127</v>
       </c>
-      <c r="G456" s="43" t="s">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="457" spans="1:7">
+      <c r="G456" s="43"/>
+    </row>
+    <row r="457" spans="1:7" ht="30">
       <c r="A457" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B457" s="39" t="s">
-        <v>739</v>
-      </c>
-      <c r="C457" s="43" t="s">
-        <v>690</v>
+        <v>740</v>
+      </c>
+      <c r="C457" s="39" t="s">
+        <v>741</v>
       </c>
       <c r="D457" s="39" t="s">
-        <v>560</v>
+        <v>1068</v>
       </c>
       <c r="E457" s="39"/>
       <c r="F457" s="39" t="s">
         <v>1127</v>
       </c>
-      <c r="G457" s="43"/>
-    </row>
-    <row r="458" spans="1:7" ht="30">
+      <c r="G457" s="39"/>
+    </row>
+    <row r="458" spans="1:7" ht="45">
       <c r="A458" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B458" s="39" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C458" s="39" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="D458" s="39" t="s">
-        <v>1068</v>
+        <v>598</v>
       </c>
       <c r="E458" s="39"/>
       <c r="F458" s="39" t="s">
@@ -16770,54 +16770,54 @@
       </c>
       <c r="G458" s="39"/>
     </row>
-    <row r="459" spans="1:7" ht="45">
+    <row r="459" spans="1:7">
       <c r="A459" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B459" s="39" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="C459" s="39" t="s">
-        <v>743</v>
-      </c>
-      <c r="D459" s="39" t="s">
-        <v>598</v>
-      </c>
+        <v>1083</v>
+      </c>
+      <c r="D459" s="39"/>
       <c r="E459" s="39"/>
       <c r="F459" s="39" t="s">
         <v>1127</v>
       </c>
       <c r="G459" s="39"/>
     </row>
-    <row r="460" spans="1:7">
+    <row r="460" spans="1:7" ht="60">
       <c r="A460" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B460" s="39" t="s">
-        <v>744</v>
+        <v>1084</v>
       </c>
       <c r="C460" s="39" t="s">
-        <v>1083</v>
-      </c>
-      <c r="D460" s="39"/>
+        <v>745</v>
+      </c>
+      <c r="D460" s="39" t="s">
+        <v>566</v>
+      </c>
       <c r="E460" s="39"/>
       <c r="F460" s="39" t="s">
         <v>1127</v>
       </c>
       <c r="G460" s="39"/>
     </row>
-    <row r="461" spans="1:7" ht="60">
+    <row r="461" spans="1:7" ht="30">
       <c r="A461" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B461" s="39" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C461" s="39" t="s">
-        <v>745</v>
+        <v>1082</v>
       </c>
       <c r="D461" s="39" t="s">
-        <v>566</v>
+        <v>700</v>
       </c>
       <c r="E461" s="39"/>
       <c r="F461" s="39" t="s">
@@ -16825,128 +16825,128 @@
       </c>
       <c r="G461" s="39"/>
     </row>
-    <row r="462" spans="1:7" ht="30">
+    <row r="462" spans="1:7">
       <c r="A462" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B462" s="39" t="s">
-        <v>1085</v>
-      </c>
-      <c r="C462" s="39" t="s">
-        <v>1082</v>
-      </c>
-      <c r="D462" s="39" t="s">
-        <v>700</v>
-      </c>
-      <c r="E462" s="39"/>
-      <c r="F462" s="39" t="s">
-        <v>1127</v>
-      </c>
-      <c r="G462" s="39"/>
+        <v>747</v>
+      </c>
+      <c r="C462" s="40" t="s">
+        <v>600</v>
+      </c>
+      <c r="D462" s="40"/>
+      <c r="E462" s="40"/>
+      <c r="F462" s="40"/>
+      <c r="G462" s="40"/>
     </row>
     <row r="463" spans="1:7">
       <c r="A463" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B463" s="39" t="s">
-        <v>747</v>
-      </c>
-      <c r="C463" s="40" t="s">
-        <v>600</v>
-      </c>
-      <c r="D463" s="40"/>
-      <c r="E463" s="40"/>
-      <c r="F463" s="40"/>
-      <c r="G463" s="40"/>
+        <v>748</v>
+      </c>
+      <c r="C463" s="43" t="s">
+        <v>602</v>
+      </c>
+      <c r="D463" s="39" t="s">
+        <v>577</v>
+      </c>
+      <c r="E463" s="39"/>
+      <c r="F463" s="39" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G463" s="43" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="464" spans="1:7">
       <c r="A464" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B464" s="39" t="s">
-        <v>748</v>
-      </c>
-      <c r="C464" s="43" t="s">
-        <v>602</v>
+        <v>749</v>
+      </c>
+      <c r="C464" s="39" t="s">
+        <v>604</v>
       </c>
       <c r="D464" s="39" t="s">
-        <v>577</v>
+        <v>1066</v>
       </c>
       <c r="E464" s="39"/>
       <c r="F464" s="39" t="s">
         <v>1127</v>
       </c>
-      <c r="G464" s="43" t="s">
-        <v>1111</v>
-      </c>
+      <c r="G464" s="39"/>
     </row>
     <row r="465" spans="1:7">
       <c r="A465" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B465" s="39" t="s">
-        <v>749</v>
-      </c>
-      <c r="C465" s="39" t="s">
-        <v>604</v>
-      </c>
-      <c r="D465" s="39" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E465" s="39"/>
-      <c r="F465" s="39" t="s">
-        <v>1127</v>
-      </c>
-      <c r="G465" s="39"/>
+        <v>750</v>
+      </c>
+      <c r="C465" s="40" t="s">
+        <v>606</v>
+      </c>
+      <c r="D465" s="40"/>
+      <c r="E465" s="40"/>
+      <c r="F465" s="40"/>
+      <c r="G465" s="40"/>
     </row>
     <row r="466" spans="1:7">
       <c r="A466" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B466" s="39" t="s">
-        <v>750</v>
-      </c>
-      <c r="C466" s="40" t="s">
-        <v>606</v>
-      </c>
-      <c r="D466" s="40"/>
-      <c r="E466" s="40"/>
-      <c r="F466" s="40"/>
-      <c r="G466" s="40"/>
-    </row>
-    <row r="467" spans="1:7">
+        <v>751</v>
+      </c>
+      <c r="C466" s="43" t="s">
+        <v>570</v>
+      </c>
+      <c r="D466" s="39" t="s">
+        <v>571</v>
+      </c>
+      <c r="E466" s="39"/>
+      <c r="F466" s="39" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G466" s="43" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="467" spans="1:7" ht="30">
       <c r="A467" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B467" s="39" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C467" s="43" t="s">
-        <v>570</v>
+        <v>645</v>
       </c>
       <c r="D467" s="39" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="E467" s="39"/>
       <c r="F467" s="39" t="s">
-        <v>1183</v>
-      </c>
-      <c r="G467" s="43" t="s">
-        <v>1120</v>
-      </c>
+        <v>1127</v>
+      </c>
+      <c r="G467" s="43"/>
     </row>
     <row r="468" spans="1:7" ht="30">
       <c r="A468" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B468" s="39" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C468" s="43" t="s">
-        <v>645</v>
+        <v>611</v>
       </c>
       <c r="D468" s="39" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="E468" s="39"/>
       <c r="F468" s="39" t="s">
@@ -16954,37 +16954,37 @@
       </c>
       <c r="G468" s="43"/>
     </row>
-    <row r="469" spans="1:7" ht="30">
+    <row r="469" spans="1:7">
       <c r="A469" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B469" s="39" t="s">
-        <v>753</v>
-      </c>
-      <c r="C469" s="43" t="s">
-        <v>611</v>
+        <v>754</v>
+      </c>
+      <c r="C469" s="39" t="s">
+        <v>613</v>
       </c>
       <c r="D469" s="39" t="s">
-        <v>577</v>
+        <v>1069</v>
       </c>
       <c r="E469" s="39"/>
       <c r="F469" s="39" t="s">
         <v>1127</v>
       </c>
-      <c r="G469" s="43"/>
-    </row>
-    <row r="470" spans="1:7">
+      <c r="G469" s="39"/>
+    </row>
+    <row r="470" spans="1:7" ht="30">
       <c r="A470" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B470" s="39" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C470" s="39" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D470" s="39" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="E470" s="39"/>
       <c r="F470" s="39" t="s">
@@ -17010,25 +17010,6 @@
         <v>1127</v>
       </c>
       <c r="G471" s="39"/>
-    </row>
-    <row r="472" spans="1:7" ht="30">
-      <c r="A472" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B472" s="39" t="s">
-        <v>755</v>
-      </c>
-      <c r="C472" s="39" t="s">
-        <v>615</v>
-      </c>
-      <c r="D472" s="39" t="s">
-        <v>1067</v>
-      </c>
-      <c r="E472" s="39"/>
-      <c r="F472" s="39" t="s">
-        <v>1127</v>
-      </c>
-      <c r="G472" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -19736,7 +19717,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:IV30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
@@ -20335,7 +20318,7 @@
   <dimension ref="A1:IV4"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -20444,7 +20427,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates to Carillon database, card auth policy oid was wrong.  Prod PIV-I cards have a deprecated tag in CHUID.  Added a line to account for that
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV-I_Carillon.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV-I_Carillon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GSA\GSA_GIT\piv-conformance-pkix-11\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045753A0-4998-497C-9B95-B4F919CE7E62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDA868F-4BFD-4661-93C6-B7778C2CBBD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -3958,13 +3958,13 @@
     <t>1.3.6.1.4.1.45606.3.1.22</t>
   </si>
   <si>
+    <t>2.16.840.1.101.3.8.7</t>
+  </si>
+  <si>
     <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,
 X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,
-X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID;1.3.6.1.4.1.45606.3.1.3:1.3.6.1.4.1.45606.3.1.4:1.3.6.1.4.1.45606.3.1.9:1.3.6.1.4.1.45606.3.1.10,
+X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID;1.3.6.1.4.1.45606.3.1.21,
 CARD_HOLDER_UNIQUE_IDENTIFIER_OID;1.3.6.1.4.1.45606.3.1.22</t>
-  </si>
-  <si>
-    <t>2.16.840.1.101.3.8.7</t>
   </si>
 </sst>
 </file>
@@ -8519,7 +8519,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G469"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A418" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A429" sqref="A429:XFD429"/>
     </sheetView>
   </sheetViews>
@@ -19991,7 +19991,7 @@
         <v>985</v>
       </c>
       <c r="E15" s="53" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="F15" s="53" t="s">
         <v>764</v>
@@ -20397,8 +20397,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -20782,7 +20782,7 @@
       </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:256" ht="315">
+    <row r="7" spans="1:256" ht="283.5">
       <c r="A7" s="6" t="s">
         <v>566</v>
       </c>
@@ -20796,7 +20796,7 @@
         <v>1019</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>764</v>

</xml_diff>